<commit_message>
ExoStar haunts your deams.
</commit_message>
<xml_diff>
--- a/vfProcGenStores/DataManagerItems.xlsx
+++ b/vfProcGenStores/DataManagerItems.xlsx
@@ -2336,24 +2336,36 @@
     <t>Ammo_AmmunitionBox_Generic_AC20_Tracer</t>
   </si>
   <si>
+    <t>emod_arm_part_shoulder</t>
+  </si>
+  <si>
     <t>emod_structureslots_standard</t>
   </si>
   <si>
     <t>emod_armorslots_standard</t>
   </si>
   <si>
+    <t>Mech_Default_Quirk</t>
+  </si>
+  <si>
+    <t>emod_arm_part_hand</t>
+  </si>
+  <si>
+    <t>emod_arm_part_lower</t>
+  </si>
+  <si>
+    <t>emod_arm_part_upper</t>
+  </si>
+  <si>
+    <t>Gear_Gyro_Generic_Standard</t>
+  </si>
+  <si>
     <t>emod_leg_hip</t>
   </si>
   <si>
     <t>Gear_Cockpit_Generic_Standard</t>
   </si>
   <si>
-    <t>emod_arm_part_shoulder</t>
-  </si>
-  <si>
-    <t>Mech_Default_Quirk</t>
-  </si>
-  <si>
     <t>emod_leg_foot</t>
   </si>
   <si>
@@ -2369,18 +2381,6 @@
     <t>Gear_Cockpit_SensorsA_Standard</t>
   </si>
   <si>
-    <t>emod_arm_part_hand</t>
-  </si>
-  <si>
-    <t>emod_arm_part_lower</t>
-  </si>
-  <si>
-    <t>emod_arm_part_upper</t>
-  </si>
-  <si>
-    <t>Gear_Gyro_Generic_Standard</t>
-  </si>
-  <si>
     <t>Gear_Actuator_Pitban_Jackrabbit</t>
   </si>
   <si>
@@ -3239,1132 +3239,1132 @@
     <t>Gear_JumpJet_Generic_Assault</t>
   </si>
   <si>
+    <t>Weapon_Laser_AI_Imaginary</t>
+  </si>
+  <si>
+    <t>Weapon_Autocannon_AC5_0-STOCK</t>
+  </si>
+  <si>
+    <t>Weapon_Laser_MediumLaser_0-STOCK</t>
+  </si>
+  <si>
+    <t>Weapon_Laser_MediumLaser_3-Starflash</t>
+  </si>
+  <si>
+    <t>Weapon_Laser_MediumLaser_3-Omicron</t>
+  </si>
+  <si>
+    <t>Weapon_Laser_MediumLaser_3-Magna</t>
+  </si>
+  <si>
+    <t>Weapon_Laser_MediumLaser_3-Intek</t>
+  </si>
+  <si>
+    <t>Weapon_Laser_MediumLaser_3-ExoStar</t>
+  </si>
+  <si>
+    <t>Weapon_Laser_MediumLaser_2-Starflash</t>
+  </si>
+  <si>
+    <t>Weapon_Laser_MediumLaser_2-Omicron</t>
+  </si>
+  <si>
+    <t>Weapon_Laser_MediumLaser_2-ExoStar</t>
+  </si>
+  <si>
+    <t>Weapon_Laser_MediumLaser_1-Starflash</t>
+  </si>
+  <si>
+    <t>Weapon_Laser_MediumLaser_1-Omicron</t>
+  </si>
+  <si>
+    <t>Weapon_Laser_MediumLaser_1-ExoStar</t>
+  </si>
+  <si>
+    <t>Weapon_Laser_MediumLaser_1-Diverse_Optics</t>
+  </si>
+  <si>
+    <t>Weapon_Laser_MediumLaser_3-Diverse_Optics</t>
+  </si>
+  <si>
+    <t>Weapon_Laser_MediumLaser_2-Magna</t>
+  </si>
+  <si>
+    <t>Weapon_Laser_MediumLaser_2-Intek</t>
+  </si>
+  <si>
+    <t>Weapon_Laser_MediumLaser_2-Diverse_Optics</t>
+  </si>
+  <si>
+    <t>Weapon_Laser_MediumLaser_1-Magna</t>
+  </si>
+  <si>
+    <t>Weapon_Laser_MediumLaser_1-Intek</t>
+  </si>
+  <si>
+    <t>Weapon_MeleeAttack</t>
+  </si>
+  <si>
+    <t>Weapon_DFAAttack</t>
+  </si>
+  <si>
+    <t>Weapon_Laser_MediumLaserPulse_0-STOCK</t>
+  </si>
+  <si>
+    <t>Weapon_Laser_MediumLaserER_0-STOCK</t>
+  </si>
+  <si>
+    <t>Weapon_Laser_LargeLaser_0-STOCK</t>
+  </si>
+  <si>
+    <t>Weapon_Laser_LargeLaserPulse_0-STOCK</t>
+  </si>
+  <si>
+    <t>Weapon_Laser_LargeLaserER_0-STOCK</t>
+  </si>
+  <si>
     <t>Weapon_LRM_LRM5_0-STOCK</t>
   </si>
   <si>
-    <t>Weapon_Autocannon_AC5_0-STOCK</t>
-  </si>
-  <si>
-    <t>Weapon_Laser_MediumLaser_0-STOCK</t>
-  </si>
-  <si>
-    <t>Weapon_Laser_MediumLaser_3-Starflash</t>
-  </si>
-  <si>
-    <t>Weapon_Laser_MediumLaser_3-Omicron</t>
-  </si>
-  <si>
-    <t>Weapon_Laser_MediumLaser_3-Magna</t>
-  </si>
-  <si>
-    <t>Weapon_Laser_MediumLaser_3-Intek</t>
-  </si>
-  <si>
-    <t>Weapon_Laser_MediumLaser_3-ExoStar</t>
-  </si>
-  <si>
-    <t>Weapon_Laser_MediumLaser_2-Starflash</t>
-  </si>
-  <si>
-    <t>Weapon_Laser_MediumLaser_2-Omicron</t>
-  </si>
-  <si>
-    <t>Weapon_Laser_MediumLaser_2-ExoStar</t>
-  </si>
-  <si>
-    <t>Weapon_Laser_MediumLaser_1-Starflash</t>
-  </si>
-  <si>
-    <t>Weapon_Laser_MediumLaser_1-Omicron</t>
-  </si>
-  <si>
-    <t>Weapon_Laser_MediumLaser_1-ExoStar</t>
-  </si>
-  <si>
-    <t>Weapon_Laser_MediumLaser_1-Diverse_Optics</t>
-  </si>
-  <si>
-    <t>Weapon_Laser_MediumLaser_3-Diverse_Optics</t>
-  </si>
-  <si>
-    <t>Weapon_Laser_MediumLaser_2-Magna</t>
-  </si>
-  <si>
-    <t>Weapon_Laser_MediumLaser_2-Intek</t>
-  </si>
-  <si>
-    <t>Weapon_Laser_MediumLaser_2-Diverse_Optics</t>
-  </si>
-  <si>
-    <t>Weapon_Laser_MediumLaser_1-Magna</t>
-  </si>
-  <si>
-    <t>Weapon_Laser_MediumLaser_1-Intek</t>
-  </si>
-  <si>
-    <t>Weapon_Laser_MediumLaserPulse_0-STOCK</t>
-  </si>
-  <si>
-    <t>Weapon_Laser_MediumLaserER_0-STOCK</t>
-  </si>
-  <si>
-    <t>Weapon_Laser_LargeLaser_0-STOCK</t>
-  </si>
-  <si>
-    <t>Weapon_Laser_LargeLaserPulse_0-STOCK</t>
-  </si>
-  <si>
-    <t>Weapon_Laser_LargeLaserER_0-STOCK</t>
-  </si>
-  <si>
-    <t>Weapon_Laser_AI_Imaginary</t>
-  </si>
-  <si>
-    <t>Weapon_MeleeAttack</t>
+    <t>Weapon_Laser_TwinSmallLaser_3-Omicron</t>
+  </si>
+  <si>
+    <t>Weapon_Laser_TwinSmallLaser_2-Magna</t>
+  </si>
+  <si>
+    <t>Weapon_Laser_TwinSmallLaser_1-ExoStar</t>
+  </si>
+  <si>
+    <t>Weapon_Laser_TwinSmallLaser_0-STOCK</t>
+  </si>
+  <si>
+    <t>Weapon_Laser_SmallLaser_3-Starflash</t>
+  </si>
+  <si>
+    <t>Weapon_Laser_SmallLaser_3-Omicron</t>
+  </si>
+  <si>
+    <t>Weapon_Laser_SmallLaser_3-Magna</t>
+  </si>
+  <si>
+    <t>Weapon_Laser_SmallLaser_3-ExoStar</t>
+  </si>
+  <si>
+    <t>Weapon_Laser_SmallLaser_3-Diverse_Optics</t>
+  </si>
+  <si>
+    <t>Weapon_Laser_SmallLaser_2-Starflash</t>
+  </si>
+  <si>
+    <t>Weapon_Laser_SmallLaser_2-Omicron</t>
+  </si>
+  <si>
+    <t>Weapon_Laser_SmallLaser_2-ExoStar</t>
+  </si>
+  <si>
+    <t>Weapon_Laser_SmallLaser_1-Starflash</t>
+  </si>
+  <si>
+    <t>Weapon_Laser_SmallLaser_1-Omicron</t>
+  </si>
+  <si>
+    <t>Weapon_Laser_SmallLaser_1-Intek</t>
+  </si>
+  <si>
+    <t>Weapon_Laser_SmallLaser_1-ExoStar</t>
+  </si>
+  <si>
+    <t>Weapon_Laser_LargeLaser_3-Starflash</t>
+  </si>
+  <si>
+    <t>Weapon_Laser_LargeLaser_3-Omicron</t>
+  </si>
+  <si>
+    <t>Weapon_Laser_LargeLaser_3-Intek</t>
+  </si>
+  <si>
+    <t>Weapon_Laser_LargeLaser_3-ExoStar</t>
+  </si>
+  <si>
+    <t>Weapon_Laser_LargeLaser_3-Diverse_Optics</t>
+  </si>
+  <si>
+    <t>Weapon_Laser_LargeLaser_2-Starflash</t>
+  </si>
+  <si>
+    <t>Weapon_Laser_LargeLaser_2-Omicron</t>
+  </si>
+  <si>
+    <t>Weapon_Laser_LargeLaser_2-ExoStar</t>
+  </si>
+  <si>
+    <t>Weapon_Laser_LargeLaser_1-Starflash</t>
+  </si>
+  <si>
+    <t>Weapon_Laser_LargeLaser_1-Omicron</t>
+  </si>
+  <si>
+    <t>Weapon_Laser_LargeLaser_1-Magna</t>
+  </si>
+  <si>
+    <t>Weapon_Laser_LargeLaser_1-ExoStar</t>
+  </si>
+  <si>
+    <t>Weapon_Laser_BinaryLaserCannon_3-Omicron</t>
+  </si>
+  <si>
+    <t>Weapon_Laser_BinaryLaserCannon_2-Magna</t>
+  </si>
+  <si>
+    <t>Weapon_Laser_BinaryLaserCannon_1-ExoStar</t>
+  </si>
+  <si>
+    <t>Weapon_Laser_BinaryLaserCannon_0-STOCK</t>
+  </si>
+  <si>
+    <t>Weapon_COIL_COIL-L_0-STOCK</t>
+  </si>
+  <si>
+    <t>Weapon_Laser_SmallLaserPulse_2-Magna200P</t>
+  </si>
+  <si>
+    <t>Weapon_Laser_SmallLaserPulse_1-Maxell</t>
+  </si>
+  <si>
+    <t>Weapon_Laser_SmallLaserER_2-BlazeFire</t>
+  </si>
+  <si>
+    <t>Weapon_Laser_SmallLaserER_1-Diverse_Optics</t>
+  </si>
+  <si>
+    <t>Weapon_Laser_MediumLaserPulse_2-Magna400P</t>
+  </si>
+  <si>
+    <t>Weapon_Laser_MediumLaserPulse_1-RakerIV</t>
+  </si>
+  <si>
+    <t>Weapon_Laser_MediumLaserER_2-BrightBloom</t>
+  </si>
+  <si>
+    <t>Weapon_Laser_MediumLaserER_1-MagnaVI</t>
+  </si>
+  <si>
+    <t>Weapon_Laser_LargeLaserPulse_2-Exostar</t>
+  </si>
+  <si>
+    <t>Weapon_Laser_LargeLaserPulse_1-Thunderbolt12</t>
+  </si>
+  <si>
+    <t>Weapon_Laser_LargeLaserER_2-BlazeFire</t>
+  </si>
+  <si>
+    <t>Weapon_Laser_LargeLaserER_1-Blankenburg25</t>
+  </si>
+  <si>
+    <t>Weapon_PPC_PPCER_0-STOCK</t>
+  </si>
+  <si>
+    <t>Weapon_Laser_SmallLaser_3-Intek</t>
+  </si>
+  <si>
+    <t>Weapon_Laser_SmallLaser_2-Magna</t>
+  </si>
+  <si>
+    <t>Weapon_Laser_SmallLaser_2-Intek</t>
+  </si>
+  <si>
+    <t>Weapon_Laser_SmallLaser_2-Diverse_Optics</t>
+  </si>
+  <si>
+    <t>Weapon_Laser_SmallLaser_1-Magna</t>
+  </si>
+  <si>
+    <t>Weapon_Laser_SmallLaser_1-Diverse_Optics</t>
+  </si>
+  <si>
+    <t>Weapon_Laser_SmallLaser_0-STOCK</t>
+  </si>
+  <si>
+    <t>Weapon_Laser_SmallLaserPulse_0-STOCK</t>
+  </si>
+  <si>
+    <t>Weapon_Laser_SmallLaserER_0-STOCK</t>
+  </si>
+  <si>
+    <t>Weapon_Laser_LargeLaser_3-Magna</t>
+  </si>
+  <si>
+    <t>Weapon_Laser_LargeLaser_2-Magna</t>
+  </si>
+  <si>
+    <t>Weapon_Laser_LargeLaser_2-Intek</t>
+  </si>
+  <si>
+    <t>Weapon_Laser_LargeLaser_2-Diverse_Optics</t>
+  </si>
+  <si>
+    <t>Weapon_Laser_LargeLaser_1-Intek</t>
+  </si>
+  <si>
+    <t>Weapon_Laser_LargeLaser_1-Diverse_Optics</t>
+  </si>
+  <si>
+    <t>Weapon_Flamer_Flamer_2-Olympus</t>
+  </si>
+  <si>
+    <t>Weapon_Flamer_Flamer_1-Hotshot</t>
+  </si>
+  <si>
+    <t>Weapon_Flamer_Flamer_0-STOCK</t>
   </si>
   <si>
     <t>Weapon_SRM_SRM2_0-STOCK</t>
   </si>
   <si>
-    <t>Weapon_Laser_LargeLaser_3-Starflash</t>
-  </si>
-  <si>
-    <t>Weapon_Laser_LargeLaser_3-Omicron</t>
-  </si>
-  <si>
-    <t>Weapon_Laser_LargeLaser_3-Intek</t>
-  </si>
-  <si>
-    <t>Weapon_Laser_LargeLaser_3-ExoStar</t>
-  </si>
-  <si>
-    <t>Weapon_Laser_LargeLaser_3-Diverse_Optics</t>
-  </si>
-  <si>
-    <t>Weapon_Laser_LargeLaser_2-Starflash</t>
-  </si>
-  <si>
-    <t>Weapon_Laser_LargeLaser_2-Omicron</t>
-  </si>
-  <si>
-    <t>Weapon_Laser_LargeLaser_2-ExoStar</t>
-  </si>
-  <si>
-    <t>Weapon_Laser_LargeLaser_1-Starflash</t>
-  </si>
-  <si>
-    <t>Weapon_Laser_LargeLaser_1-Omicron</t>
-  </si>
-  <si>
-    <t>Weapon_Laser_LargeLaser_1-Magna</t>
-  </si>
-  <si>
-    <t>Weapon_Laser_LargeLaser_1-ExoStar</t>
-  </si>
-  <si>
-    <t>Weapon_Laser_BinaryLaserCannon_3-Omicron</t>
-  </si>
-  <si>
-    <t>Weapon_Laser_BinaryLaserCannon_2-Magna</t>
-  </si>
-  <si>
-    <t>Weapon_Laser_BinaryLaserCannon_1-ExoStar</t>
-  </si>
-  <si>
-    <t>Weapon_Laser_BinaryLaserCannon_0-STOCK</t>
-  </si>
-  <si>
-    <t>Weapon_COIL_COIL-L_0-STOCK</t>
-  </si>
-  <si>
-    <t>Weapon_Laser_MediumLaserPulse_2-Magna400P</t>
-  </si>
-  <si>
-    <t>Weapon_Laser_MediumLaserPulse_1-RakerIV</t>
-  </si>
-  <si>
-    <t>Weapon_Laser_MediumLaserER_2-BrightBloom</t>
-  </si>
-  <si>
-    <t>Weapon_Laser_MediumLaserER_1-MagnaVI</t>
-  </si>
-  <si>
-    <t>Weapon_Laser_LargeLaserPulse_2-Exostar</t>
-  </si>
-  <si>
-    <t>Weapon_Laser_LargeLaserPulse_1-Thunderbolt12</t>
-  </si>
-  <si>
-    <t>Weapon_Laser_LargeLaserER_2-BlazeFire</t>
-  </si>
-  <si>
-    <t>Weapon_Laser_LargeLaserER_1-Blankenburg25</t>
-  </si>
-  <si>
-    <t>Weapon_Laser_LargeLaser_3-Magna</t>
-  </si>
-  <si>
-    <t>Weapon_Laser_LargeLaser_2-Magna</t>
-  </si>
-  <si>
-    <t>Weapon_Laser_LargeLaser_2-Intek</t>
-  </si>
-  <si>
-    <t>Weapon_Laser_LargeLaser_2-Diverse_Optics</t>
-  </si>
-  <si>
-    <t>Weapon_Laser_LargeLaser_1-Intek</t>
-  </si>
-  <si>
-    <t>Weapon_Laser_LargeLaser_1-Diverse_Optics</t>
-  </si>
-  <si>
-    <t>Weapon_DFAAttack</t>
+    <t>Weapon_SRM_SSRM6_3-Valiant</t>
+  </si>
+  <si>
+    <t>Weapon_SRM_SSRM6_2-Valiant</t>
+  </si>
+  <si>
+    <t>Weapon_SRM_SSRM6_2-Irian</t>
+  </si>
+  <si>
+    <t>Weapon_SRM_SSRM6_2-Holly</t>
+  </si>
+  <si>
+    <t>Weapon_SRM_SSRM6_1-Irian</t>
+  </si>
+  <si>
+    <t>Weapon_SRM_SSRM6_1-Holly</t>
+  </si>
+  <si>
+    <t>Weapon_SRM_SSRM6_0-STOCK</t>
+  </si>
+  <si>
+    <t>Weapon_SRM_SSRM4_3-Valiant</t>
+  </si>
+  <si>
+    <t>Weapon_SRM_SSRM4_2-Valiant</t>
+  </si>
+  <si>
+    <t>Weapon_SRM_SSRM4_2-Irian</t>
+  </si>
+  <si>
+    <t>Weapon_SRM_SSRM4_2-Holly</t>
+  </si>
+  <si>
+    <t>Weapon_SRM_SSRM4_1-Irian</t>
+  </si>
+  <si>
+    <t>Weapon_SRM_SSRM4_1-Holly</t>
+  </si>
+  <si>
+    <t>Weapon_SRM_SSRM4_0-STOCK</t>
+  </si>
+  <si>
+    <t>Weapon_SRM_SSRM2_3-Valiant</t>
+  </si>
+  <si>
+    <t>Weapon_SRM_SSRM2_2-Valiant</t>
+  </si>
+  <si>
+    <t>Weapon_SRM_SSRM2_2-Irian</t>
+  </si>
+  <si>
+    <t>Weapon_SRM_SSRM2_2-Holly</t>
+  </si>
+  <si>
+    <t>Weapon_SRM_SSRM2_1-Irian</t>
+  </si>
+  <si>
+    <t>Weapon_SRM_SSRM2_1-Holly</t>
+  </si>
+  <si>
+    <t>Weapon_SRM_SSRM2_0-STOCK</t>
+  </si>
+  <si>
+    <t>Weapon_SRM_SRM6_3-Lockheed</t>
+  </si>
+  <si>
+    <t>Weapon_SRM_SRM6_3-Irian</t>
+  </si>
+  <si>
+    <t>Weapon_SRM_SRM6_3-Holly</t>
+  </si>
+  <si>
+    <t>Weapon_SRM_SRM6_3-Harvester</t>
+  </si>
+  <si>
+    <t>Weapon_SRM_SRM6_3-Coventry</t>
+  </si>
+  <si>
+    <t>Weapon_SRM_SRM6_2-Lockheed</t>
+  </si>
+  <si>
+    <t>Weapon_SRM_SRM6_2-Harvester</t>
+  </si>
+  <si>
+    <t>Weapon_SRM_SRM6_2-Coventry</t>
+  </si>
+  <si>
+    <t>Weapon_SRM_SRM6_1-Valiant</t>
+  </si>
+  <si>
+    <t>Weapon_SRM_SRM6_1-Lockheed</t>
+  </si>
+  <si>
+    <t>Weapon_SRM_SRM6_1-Harvester</t>
+  </si>
+  <si>
+    <t>Weapon_SRM_SRM6_1-Coventry</t>
+  </si>
+  <si>
+    <t>Weapon_SRM_SRM4_3-Lockheed</t>
+  </si>
+  <si>
+    <t>Weapon_SRM_SRM4_3-Irian</t>
+  </si>
+  <si>
+    <t>Weapon_SRM_SRM4_3-Holly</t>
+  </si>
+  <si>
+    <t>Weapon_SRM_SRM4_3-Harvester</t>
+  </si>
+  <si>
+    <t>Weapon_SRM_SRM4_3-Coventry</t>
+  </si>
+  <si>
+    <t>Weapon_SRM_SRM4_2-Lockheed</t>
+  </si>
+  <si>
+    <t>Weapon_SRM_SRM4_2-Harvester</t>
+  </si>
+  <si>
+    <t>Weapon_SRM_SRM4_2-Coventry</t>
+  </si>
+  <si>
+    <t>Weapon_SRM_SRM4_1-Valiant</t>
+  </si>
+  <si>
+    <t>Weapon_SRM_SRM4_1-Lockheed</t>
+  </si>
+  <si>
+    <t>Weapon_SRM_SRM4_1-Harvester</t>
+  </si>
+  <si>
+    <t>Weapon_SRM_SRM4_1-Coventry</t>
+  </si>
+  <si>
+    <t>Weapon_SRM_SRM2_3-Lockheed</t>
+  </si>
+  <si>
+    <t>Weapon_SRM_SRM2_3-Irian</t>
+  </si>
+  <si>
+    <t>Weapon_SRM_SRM2_3-Holly</t>
+  </si>
+  <si>
+    <t>Weapon_SRM_SRM2_3-Harvester</t>
+  </si>
+  <si>
+    <t>Weapon_SRM_SRM2_3-Coventry</t>
+  </si>
+  <si>
+    <t>Weapon_SRM_SRM2_2-Lockheed</t>
+  </si>
+  <si>
+    <t>Weapon_SRM_SRM2_2-Harvester</t>
+  </si>
+  <si>
+    <t>Weapon_SRM_SRM2_2-Coventry</t>
+  </si>
+  <si>
+    <t>Weapon_SRM_SRM2_1-Valiant</t>
+  </si>
+  <si>
+    <t>Weapon_SRM_SRM2_1-Lockheed</t>
+  </si>
+  <si>
+    <t>Weapon_SRM_SRM2_1-Harvester</t>
+  </si>
+  <si>
+    <t>Weapon_SRM_SRM2_1-Coventry</t>
+  </si>
+  <si>
+    <t>Weapon_PPC_PPCSnub_2-Magna</t>
+  </si>
+  <si>
+    <t>Weapon_PPC_PPCSnub_2-Donal</t>
+  </si>
+  <si>
+    <t>Weapon_PPC_PPCSnub_2-Ceres_Arms</t>
+  </si>
+  <si>
+    <t>Weapon_PPC_PPCSnub_1-Magna</t>
+  </si>
+  <si>
+    <t>Weapon_PPC_PPCSnub_1-Donal</t>
+  </si>
+  <si>
+    <t>Weapon_PPC_PPCSnub_1-Ceres_Arms</t>
+  </si>
+  <si>
+    <t>Weapon_PPC_PPCSnub_0-STOCK</t>
+  </si>
+  <si>
+    <t>Weapon_Narc_Standard_0-STOCK</t>
+  </si>
+  <si>
+    <t>Weapon_Mortar_MechMortar</t>
+  </si>
+  <si>
+    <t>Weapon_MachineGun_TwinMachineGun_2-Brigadier</t>
+  </si>
+  <si>
+    <t>Weapon_MachineGun_TwinMachineGun_1-VMI</t>
+  </si>
+  <si>
+    <t>Weapon_MachineGun_TwinMachineGun_0-STOCK</t>
+  </si>
+  <si>
+    <t>Weapon_LRM_LRM5_3-Telos</t>
+  </si>
+  <si>
+    <t>Weapon_LRM_LRM5_3-Drago</t>
+  </si>
+  <si>
+    <t>Weapon_LRM_LRM5_3-Delta</t>
+  </si>
+  <si>
+    <t>Weapon_LRM_LRM5_3-Coventry</t>
+  </si>
+  <si>
+    <t>Weapon_LRM_LRM5_3-Concordat</t>
+  </si>
+  <si>
+    <t>Weapon_LRM_LRM5_2-Drago</t>
+  </si>
+  <si>
+    <t>Weapon_LRM_LRM5_2-Coventry</t>
+  </si>
+  <si>
+    <t>Weapon_LRM_LRM5_2-Concordat</t>
+  </si>
+  <si>
+    <t>Weapon_LRM_LRM5_1-Zeus</t>
+  </si>
+  <si>
+    <t>Weapon_LRM_LRM5_1-Drago</t>
+  </si>
+  <si>
+    <t>Weapon_LRM_LRM5_1-Coventry</t>
+  </si>
+  <si>
+    <t>Weapon_LRM_LRM5_1-Concordat</t>
+  </si>
+  <si>
+    <t>Weapon_LRM_LRM20_3-Telos</t>
+  </si>
+  <si>
+    <t>Weapon_LRM_LRM20_3-Drago</t>
+  </si>
+  <si>
+    <t>Weapon_LRM_LRM20_3-Delta</t>
+  </si>
+  <si>
+    <t>Weapon_LRM_LRM20_3-Coventry</t>
+  </si>
+  <si>
+    <t>Weapon_LRM_LRM20_3-Concordat</t>
+  </si>
+  <si>
+    <t>Weapon_LRM_LRM20_2-Drago</t>
+  </si>
+  <si>
+    <t>Weapon_LRM_LRM20_2-Coventry</t>
+  </si>
+  <si>
+    <t>Weapon_LRM_LRM20_2-Concordat</t>
+  </si>
+  <si>
+    <t>Weapon_LRM_LRM20_1-Zeus</t>
+  </si>
+  <si>
+    <t>Weapon_LRM_LRM20_1-Drago</t>
+  </si>
+  <si>
+    <t>Weapon_LRM_LRM20_1-Coventry</t>
+  </si>
+  <si>
+    <t>Weapon_LRM_LRM20_1-Concordat</t>
+  </si>
+  <si>
+    <t>Weapon_LRM_LRM15_3-Telos</t>
+  </si>
+  <si>
+    <t>Weapon_LRM_LRM15_3-Drago</t>
+  </si>
+  <si>
+    <t>Weapon_LRM_LRM15_3-Delta</t>
+  </si>
+  <si>
+    <t>Weapon_LRM_LRM15_3-Coventry</t>
+  </si>
+  <si>
+    <t>Weapon_LRM_LRM15_3-Concordat</t>
+  </si>
+  <si>
+    <t>Weapon_LRM_LRM15_2-Drago</t>
+  </si>
+  <si>
+    <t>Weapon_LRM_LRM15_2-Coventry</t>
+  </si>
+  <si>
+    <t>Weapon_LRM_LRM15_2-Concordat</t>
+  </si>
+  <si>
+    <t>Weapon_LRM_LRM15_1-Zeus</t>
+  </si>
+  <si>
+    <t>Weapon_LRM_LRM15_1-Drago</t>
+  </si>
+  <si>
+    <t>Weapon_LRM_LRM15_1-Coventry</t>
+  </si>
+  <si>
+    <t>Weapon_LRM_LRM15_1-Concordat</t>
+  </si>
+  <si>
+    <t>Weapon_LRM_LRM10_3-Telos</t>
+  </si>
+  <si>
+    <t>Weapon_LRM_LRM10_3-Drago</t>
+  </si>
+  <si>
+    <t>Weapon_LRM_LRM10_3-Delta</t>
+  </si>
+  <si>
+    <t>Weapon_LRM_LRM10_3-Coventry</t>
+  </si>
+  <si>
+    <t>Weapon_LRM_LRM10_3-Concordat</t>
+  </si>
+  <si>
+    <t>Weapon_LRM_LRM10_2-Drago</t>
+  </si>
+  <si>
+    <t>Weapon_LRM_LRM10_2-Coventry</t>
+  </si>
+  <si>
+    <t>Weapon_LRM_LRM10_2-Concordat</t>
+  </si>
+  <si>
+    <t>Weapon_LRM_LRM10_1-Zeus</t>
+  </si>
+  <si>
+    <t>Weapon_LRM_LRM10_1-Drago</t>
+  </si>
+  <si>
+    <t>Weapon_LRM_LRM10_1-Coventry</t>
+  </si>
+  <si>
+    <t>Weapon_LRM_LRM10_1-Concordat</t>
+  </si>
+  <si>
+    <t>Weapon_COIL_COIL-S_0-STOCK</t>
   </si>
   <si>
     <t>Weapon_COIL_COIL-M_0-STOCK</t>
   </si>
   <si>
-    <t>Weapon_Mortar_MechMortar</t>
-  </si>
-  <si>
-    <t>Weapon_PPC_PPCER_0-STOCK</t>
+    <t>Weapon_Autocannon_UAC5_2-Mydron</t>
+  </si>
+  <si>
+    <t>Weapon_Autocannon_UAC5_1-Mydron</t>
+  </si>
+  <si>
+    <t>Weapon_Autocannon_UAC5_0-STOCK</t>
+  </si>
+  <si>
+    <t>Weapon_Autocannon_UAC2_2-Imperator</t>
+  </si>
+  <si>
+    <t>Weapon_Autocannon_UAC2_1-Imperator</t>
+  </si>
+  <si>
+    <t>Weapon_Autocannon_UAC2_0-STOCK</t>
+  </si>
+  <si>
+    <t>Weapon_Autocannon_UAC10_2-Federated</t>
+  </si>
+  <si>
+    <t>Weapon_Autocannon_UAC10_1-Federated</t>
+  </si>
+  <si>
+    <t>Weapon_Autocannon_UAC10_0-STOCK</t>
+  </si>
+  <si>
+    <t>Weapon_Autocannon_LB5X_2-GM</t>
+  </si>
+  <si>
+    <t>Weapon_Autocannon_LB5X_1-GM</t>
+  </si>
+  <si>
+    <t>Weapon_Autocannon_LB5X_0-STOCK</t>
+  </si>
+  <si>
+    <t>Weapon_Autocannon_LB2X_2-Defiance</t>
+  </si>
+  <si>
+    <t>Weapon_Autocannon_LB2X_1-Defiance</t>
+  </si>
+  <si>
+    <t>Weapon_Autocannon_LB2X_0-STOCK</t>
+  </si>
+  <si>
+    <t>Weapon_Autocannon_LB20X_2-Shengli_Arms</t>
+  </si>
+  <si>
+    <t>Weapon_Autocannon_LB20X_2-Imperator</t>
+  </si>
+  <si>
+    <t>Weapon_Autocannon_LB20X_1-Shengli_Arms</t>
+  </si>
+  <si>
+    <t>Weapon_Autocannon_LB20X_0-STOCK</t>
+  </si>
+  <si>
+    <t>Weapon_Autocannon_LB10X_2-Western</t>
+  </si>
+  <si>
+    <t>Weapon_Autocannon_LB10X_1-Western</t>
+  </si>
+  <si>
+    <t>Weapon_Autocannon_LB10X_0-STOCK</t>
+  </si>
+  <si>
+    <t>Weapon_Autocannon_AC5_3-ZeusBolt</t>
+  </si>
+  <si>
+    <t>Weapon_Autocannon_AC5_3-Kali_Yama</t>
+  </si>
+  <si>
+    <t>Weapon_Autocannon_AC5_3-Imperator</t>
+  </si>
+  <si>
+    <t>Weapon_Autocannon_AC5_3-Federated</t>
+  </si>
+  <si>
+    <t>Weapon_Autocannon_AC5_3-Defiance</t>
+  </si>
+  <si>
+    <t>Weapon_Autocannon_AC5_2-ZeusBolt</t>
+  </si>
+  <si>
+    <t>Weapon_Autocannon_AC5_1-ZeusBolt</t>
+  </si>
+  <si>
+    <t>Weapon_Autocannon_AC5_1-Mydron</t>
+  </si>
+  <si>
+    <t>Weapon_Autocannon_AC2_3-ZeusBolt</t>
+  </si>
+  <si>
+    <t>Weapon_Autocannon_AC2_3-Mydron</t>
+  </si>
+  <si>
+    <t>Weapon_Autocannon_AC2_3-Kali_Yama</t>
+  </si>
+  <si>
+    <t>Weapon_Autocannon_AC2_3-Federated</t>
+  </si>
+  <si>
+    <t>Weapon_Autocannon_AC2_3-Defiance</t>
+  </si>
+  <si>
+    <t>Weapon_Autocannon_AC2_2-ZeusBolt</t>
+  </si>
+  <si>
+    <t>Weapon_Autocannon_AC2_1-ZeusBolt</t>
+  </si>
+  <si>
+    <t>Weapon_Autocannon_AC2_1-Imperator</t>
+  </si>
+  <si>
+    <t>Weapon_Autocannon_AC10_3-ZeusBolt</t>
+  </si>
+  <si>
+    <t>Weapon_Autocannon_AC10_3-Mydron</t>
+  </si>
+  <si>
+    <t>Weapon_Autocannon_AC10_3-Kali_Yama</t>
+  </si>
+  <si>
+    <t>Weapon_Autocannon_AC10_3-Imperator</t>
+  </si>
+  <si>
+    <t>Weapon_Autocannon_AC10_3-Defiance</t>
+  </si>
+  <si>
+    <t>Weapon_Autocannon_AC10_2-ZeusBolt</t>
+  </si>
+  <si>
+    <t>Weapon_Autocannon_AC10_1-ZeusBolt</t>
+  </si>
+  <si>
+    <t>Weapon_Autocannon_AC10_1-Federated</t>
+  </si>
+  <si>
+    <t>Weapon_AMS_2</t>
+  </si>
+  <si>
+    <t>Weapon_AMS_1</t>
+  </si>
+  <si>
+    <t>Weapon_AMS</t>
+  </si>
+  <si>
+    <t>Weapon_MachineGun_MachineGun_2-VMI</t>
+  </si>
+  <si>
+    <t>Weapon_MachineGun_MachineGun_2-Brigadier</t>
+  </si>
+  <si>
+    <t>Weapon_MachineGun_MachineGun_1-VMI</t>
+  </si>
+  <si>
+    <t>Weapon_MachineGun_MachineGun_1-Brigadier</t>
+  </si>
+  <si>
+    <t>Weapon_Flamer_Flamer_SPECIAL-Victoria</t>
+  </si>
+  <si>
+    <t>Weapon_PPC_PPCER_2-TiegartMagnum</t>
+  </si>
+  <si>
+    <t>Weapon_PPC_PPCER_1-MagnaFirestar</t>
+  </si>
+  <si>
+    <t>Weapon_Gauss_Gauss_2-M9</t>
+  </si>
+  <si>
+    <t>Weapon_Gauss_Gauss_1-M7</t>
+  </si>
+  <si>
+    <t>Weapon_SRM_SRM6_3-Valiant</t>
+  </si>
+  <si>
+    <t>Weapon_SRM_SRM6_2-Valiant</t>
+  </si>
+  <si>
+    <t>Weapon_SRM_SRM6_2-Irian</t>
+  </si>
+  <si>
+    <t>Weapon_SRM_SRM6_2-Holly</t>
+  </si>
+  <si>
+    <t>Weapon_SRM_SRM6_1-Irian</t>
+  </si>
+  <si>
+    <t>Weapon_SRM_SRM6_1-Holly</t>
+  </si>
+  <si>
+    <t>Weapon_SRM_SRM6_0-STOCK</t>
+  </si>
+  <si>
+    <t>Weapon_SRM_SRM4_3-Valiant</t>
+  </si>
+  <si>
+    <t>Weapon_SRM_SRM4_2-Valiant</t>
+  </si>
+  <si>
+    <t>Weapon_SRM_SRM4_2-Irian</t>
+  </si>
+  <si>
+    <t>Weapon_SRM_SRM4_2-Holly</t>
+  </si>
+  <si>
+    <t>Weapon_SRM_SRM4_1-Irian</t>
+  </si>
+  <si>
+    <t>Weapon_SRM_SRM4_1-Holly</t>
+  </si>
+  <si>
+    <t>Weapon_SRM_SRM4_0-STOCK</t>
+  </si>
+  <si>
+    <t>Weapon_SRM_SRM2_3-Valiant</t>
+  </si>
+  <si>
+    <t>Weapon_SRM_SRM2_2-Valiant</t>
+  </si>
+  <si>
+    <t>Weapon_SRM_SRM2_2-Irian</t>
+  </si>
+  <si>
+    <t>Weapon_SRM_SRM2_2-Holly</t>
+  </si>
+  <si>
+    <t>Weapon_SRM_SRM2_1-Irian</t>
+  </si>
+  <si>
+    <t>Weapon_SRM_SRM2_1-Holly</t>
+  </si>
+  <si>
+    <t>Weapon_PPC_PPC_2-Tiegart</t>
+  </si>
+  <si>
+    <t>Weapon_PPC_PPC_2-Donal</t>
+  </si>
+  <si>
+    <t>Weapon_PPC_PPC_2-Ceres_Arms</t>
+  </si>
+  <si>
+    <t>Weapon_PPC_PPC_1-Tiegart</t>
+  </si>
+  <si>
+    <t>Weapon_PPC_PPC_1-Donal</t>
+  </si>
+  <si>
+    <t>Weapon_PPC_PPC_1-Ceres_Arms</t>
+  </si>
+  <si>
+    <t>Weapon_PPC_PPC_0-STOCK</t>
+  </si>
+  <si>
+    <t>Weapon_MachineGun_MachineGun_0-STOCK</t>
+  </si>
+  <si>
+    <t>Weapon_LRM_LRM5_3-Zeus</t>
+  </si>
+  <si>
+    <t>Weapon_LRM_LRM5_2-Zeus</t>
+  </si>
+  <si>
+    <t>Weapon_LRM_LRM5_2-Telos</t>
+  </si>
+  <si>
+    <t>Weapon_LRM_LRM5_2-LongFire</t>
+  </si>
+  <si>
+    <t>Weapon_LRM_LRM5_2-Delta</t>
+  </si>
+  <si>
+    <t>Weapon_LRM_LRM5_1-Telos</t>
+  </si>
+  <si>
+    <t>Weapon_LRM_LRM5_1-LongFire</t>
+  </si>
+  <si>
+    <t>Weapon_LRM_LRM5_1-Delta</t>
+  </si>
+  <si>
+    <t>Weapon_LRM_LRM20_3-Zeus</t>
+  </si>
+  <si>
+    <t>Weapon_LRM_LRM20_2-Zeus</t>
+  </si>
+  <si>
+    <t>Weapon_LRM_LRM20_2-Telos</t>
+  </si>
+  <si>
+    <t>Weapon_LRM_LRM20_2-LongFire</t>
+  </si>
+  <si>
+    <t>Weapon_LRM_LRM20_2-Delta</t>
+  </si>
+  <si>
+    <t>Weapon_LRM_LRM20_1-Telos</t>
+  </si>
+  <si>
+    <t>Weapon_LRM_LRM20_1-LongFire</t>
+  </si>
+  <si>
+    <t>Weapon_LRM_LRM20_1-Delta</t>
+  </si>
+  <si>
+    <t>Weapon_LRM_LRM20_0-STOCK</t>
+  </si>
+  <si>
+    <t>Weapon_LRM_LRM15_3-Zeus</t>
+  </si>
+  <si>
+    <t>Weapon_LRM_LRM15_2-Zeus</t>
+  </si>
+  <si>
+    <t>Weapon_LRM_LRM15_2-Telos</t>
+  </si>
+  <si>
+    <t>Weapon_LRM_LRM15_2-LongFire</t>
+  </si>
+  <si>
+    <t>Weapon_LRM_LRM15_2-Delta</t>
+  </si>
+  <si>
+    <t>Weapon_LRM_LRM15_1-Telos</t>
+  </si>
+  <si>
+    <t>Weapon_LRM_LRM15_1-LongFire</t>
+  </si>
+  <si>
+    <t>Weapon_LRM_LRM15_1-Delta</t>
+  </si>
+  <si>
+    <t>Weapon_LRM_LRM15_0-STOCK</t>
+  </si>
+  <si>
+    <t>Weapon_LRM_LRM10_3-Zeus</t>
+  </si>
+  <si>
+    <t>Weapon_LRM_LRM10_2-Zeus</t>
+  </si>
+  <si>
+    <t>Weapon_LRM_LRM10_2-Telos</t>
+  </si>
+  <si>
+    <t>Weapon_LRM_LRM10_2-LongFire</t>
+  </si>
+  <si>
+    <t>Weapon_LRM_LRM10_2-Delta</t>
+  </si>
+  <si>
+    <t>Weapon_LRM_LRM10_1-Telos</t>
+  </si>
+  <si>
+    <t>Weapon_LRM_LRM10_1-LongFire</t>
+  </si>
+  <si>
+    <t>Weapon_LRM_LRM10_1-Delta</t>
+  </si>
+  <si>
+    <t>Weapon_LRM_LRM10_0-STOCK</t>
+  </si>
+  <si>
+    <t>Weapon_Gauss_Gauss_0-STOCK</t>
+  </si>
+  <si>
+    <t>Weapon_Autocannon_AC5_3-Mydron</t>
+  </si>
+  <si>
+    <t>Weapon_Autocannon_AC5_2-Mydron</t>
+  </si>
+  <si>
+    <t>Weapon_Autocannon_AC5_2-Kali_Yama</t>
+  </si>
+  <si>
+    <t>Weapon_Autocannon_AC5_2-Imperator</t>
+  </si>
+  <si>
+    <t>Weapon_Autocannon_AC5_2-Federated</t>
+  </si>
+  <si>
+    <t>Weapon_Autocannon_AC5_2-Defiance</t>
+  </si>
+  <si>
+    <t>Weapon_Autocannon_AC5_1-Kali_Yama</t>
+  </si>
+  <si>
+    <t>Weapon_Autocannon_AC5_1-Imperator</t>
+  </si>
+  <si>
+    <t>Weapon_Autocannon_AC5_1-Federated</t>
+  </si>
+  <si>
+    <t>Weapon_Autocannon_AC5_1-Defiance</t>
+  </si>
+  <si>
+    <t>Weapon_Autocannon_AC2_3-Imperator</t>
+  </si>
+  <si>
+    <t>Weapon_Autocannon_AC2_2-Mydron</t>
+  </si>
+  <si>
+    <t>Weapon_Autocannon_AC2_2-Kali_Yama</t>
+  </si>
+  <si>
+    <t>Weapon_Autocannon_AC2_2-Imperator</t>
+  </si>
+  <si>
+    <t>Weapon_Autocannon_AC2_2-Federated</t>
+  </si>
+  <si>
+    <t>Weapon_Autocannon_AC2_2-Defiance</t>
+  </si>
+  <si>
+    <t>Weapon_Autocannon_AC2_1-Mydron</t>
+  </si>
+  <si>
+    <t>Weapon_Autocannon_AC2_1-Kali_Yama</t>
+  </si>
+  <si>
+    <t>Weapon_Autocannon_AC2_1-Federated</t>
+  </si>
+  <si>
+    <t>Weapon_Autocannon_AC2_1-Defiance</t>
+  </si>
+  <si>
+    <t>Weapon_Autocannon_AC2_0-STOCK</t>
+  </si>
+  <si>
+    <t>Weapon_Autocannon_AC10_3-Federated</t>
+  </si>
+  <si>
+    <t>Weapon_Autocannon_AC10_2-Mydron</t>
+  </si>
+  <si>
+    <t>Weapon_Autocannon_AC10_2-Kali_Yama</t>
+  </si>
+  <si>
+    <t>Weapon_Autocannon_AC10_2-Imperator</t>
+  </si>
+  <si>
+    <t>Weapon_Autocannon_AC10_2-Federated</t>
+  </si>
+  <si>
+    <t>Weapon_Autocannon_AC10_2-Defiance</t>
+  </si>
+  <si>
+    <t>Weapon_Autocannon_AC10_1-Mydron</t>
+  </si>
+  <si>
+    <t>Weapon_Autocannon_AC10_1-Kali_Yama</t>
+  </si>
+  <si>
+    <t>Weapon_Autocannon_AC10_1-Imperator</t>
+  </si>
+  <si>
+    <t>Weapon_Autocannon_AC10_1-Defiance</t>
+  </si>
+  <si>
+    <t>Weapon_Autocannon_AC10_0-STOCK</t>
+  </si>
+  <si>
+    <t>Weapon_Inferno_Inferno2_2-Marklin_Mini</t>
+  </si>
+  <si>
+    <t>Weapon_Inferno_Inferno2_1-Harvester</t>
+  </si>
+  <si>
+    <t>Weapon_Inferno_Inferno2_0-STOCK</t>
+  </si>
+  <si>
+    <t>Weapon_TAG_Standard_2-Ceres_Arms</t>
+  </si>
+  <si>
+    <t>Weapon_TAG_Standard_1-Mendham</t>
   </si>
   <si>
     <t>Weapon_TAG_Standard_0-STOCK</t>
   </si>
   <si>
-    <t>Weapon_PPC_PPCSnub_0-STOCK</t>
+    <t>Weapon_Narc_Standard_2-Kali_Yama</t>
+  </si>
+  <si>
+    <t>Weapon_Narc_Standard_1-Ceres_Arms</t>
   </si>
   <si>
     <t>Weapon_Mortar_Thumper</t>
-  </si>
-  <si>
-    <t>Weapon_Laser_TwinSmallLaser_3-Omicron</t>
-  </si>
-  <si>
-    <t>Weapon_Laser_TwinSmallLaser_2-Magna</t>
-  </si>
-  <si>
-    <t>Weapon_Laser_TwinSmallLaser_1-ExoStar</t>
-  </si>
-  <si>
-    <t>Weapon_Laser_TwinSmallLaser_0-STOCK</t>
-  </si>
-  <si>
-    <t>Weapon_Laser_SmallLaser_3-Starflash</t>
-  </si>
-  <si>
-    <t>Weapon_Laser_SmallLaser_3-Omicron</t>
-  </si>
-  <si>
-    <t>Weapon_Laser_SmallLaser_3-Magna</t>
-  </si>
-  <si>
-    <t>Weapon_Laser_SmallLaser_3-ExoStar</t>
-  </si>
-  <si>
-    <t>Weapon_Laser_SmallLaser_3-Diverse_Optics</t>
-  </si>
-  <si>
-    <t>Weapon_Laser_SmallLaser_2-Starflash</t>
-  </si>
-  <si>
-    <t>Weapon_Laser_SmallLaser_2-Omicron</t>
-  </si>
-  <si>
-    <t>Weapon_Laser_SmallLaser_2-ExoStar</t>
-  </si>
-  <si>
-    <t>Weapon_Laser_SmallLaser_1-Starflash</t>
-  </si>
-  <si>
-    <t>Weapon_Laser_SmallLaser_1-Omicron</t>
-  </si>
-  <si>
-    <t>Weapon_Laser_SmallLaser_1-Intek</t>
-  </si>
-  <si>
-    <t>Weapon_Laser_SmallLaser_1-ExoStar</t>
-  </si>
-  <si>
-    <t>Weapon_COIL_COIL-S_0-STOCK</t>
-  </si>
-  <si>
-    <t>Weapon_Flamer_Flamer_SPECIAL-Victoria</t>
-  </si>
-  <si>
-    <t>Weapon_PPC_PPCER_2-TiegartMagnum</t>
-  </si>
-  <si>
-    <t>Weapon_PPC_PPCER_1-MagnaFirestar</t>
-  </si>
-  <si>
-    <t>Weapon_Laser_SmallLaserPulse_2-Magna200P</t>
-  </si>
-  <si>
-    <t>Weapon_Laser_SmallLaserPulse_1-Maxell</t>
-  </si>
-  <si>
-    <t>Weapon_Laser_SmallLaserER_2-BlazeFire</t>
-  </si>
-  <si>
-    <t>Weapon_Laser_SmallLaserER_1-Diverse_Optics</t>
-  </si>
-  <si>
-    <t>Weapon_PPC_PPC_2-Tiegart</t>
-  </si>
-  <si>
-    <t>Weapon_PPC_PPC_2-Donal</t>
-  </si>
-  <si>
-    <t>Weapon_PPC_PPC_2-Ceres_Arms</t>
-  </si>
-  <si>
-    <t>Weapon_PPC_PPC_1-Tiegart</t>
-  </si>
-  <si>
-    <t>Weapon_PPC_PPC_1-Donal</t>
-  </si>
-  <si>
-    <t>Weapon_PPC_PPC_1-Ceres_Arms</t>
-  </si>
-  <si>
-    <t>Weapon_PPC_PPC_0-STOCK</t>
-  </si>
-  <si>
-    <t>Weapon_Laser_SmallLaser_3-Intek</t>
-  </si>
-  <si>
-    <t>Weapon_Laser_SmallLaser_2-Magna</t>
-  </si>
-  <si>
-    <t>Weapon_Laser_SmallLaser_2-Intek</t>
-  </si>
-  <si>
-    <t>Weapon_Laser_SmallLaser_2-Diverse_Optics</t>
-  </si>
-  <si>
-    <t>Weapon_Laser_SmallLaser_1-Magna</t>
-  </si>
-  <si>
-    <t>Weapon_Laser_SmallLaser_1-Diverse_Optics</t>
-  </si>
-  <si>
-    <t>Weapon_Laser_SmallLaser_0-STOCK</t>
-  </si>
-  <si>
-    <t>Weapon_Laser_SmallLaserPulse_0-STOCK</t>
-  </si>
-  <si>
-    <t>Weapon_Laser_SmallLaserER_0-STOCK</t>
-  </si>
-  <si>
-    <t>Weapon_Flamer_Flamer_2-Olympus</t>
-  </si>
-  <si>
-    <t>Weapon_Flamer_Flamer_1-Hotshot</t>
-  </si>
-  <si>
-    <t>Weapon_Flamer_Flamer_0-STOCK</t>
-  </si>
-  <si>
-    <t>Weapon_Inferno_Inferno2_2-Marklin_Mini</t>
-  </si>
-  <si>
-    <t>Weapon_Inferno_Inferno2_1-Harvester</t>
-  </si>
-  <si>
-    <t>Weapon_Inferno_Inferno2_0-STOCK</t>
-  </si>
-  <si>
-    <t>Weapon_TAG_Standard_2-Ceres_Arms</t>
-  </si>
-  <si>
-    <t>Weapon_TAG_Standard_1-Mendham</t>
-  </si>
-  <si>
-    <t>Weapon_SRM_SSRM6_3-Valiant</t>
-  </si>
-  <si>
-    <t>Weapon_SRM_SSRM6_2-Valiant</t>
-  </si>
-  <si>
-    <t>Weapon_SRM_SSRM6_2-Irian</t>
-  </si>
-  <si>
-    <t>Weapon_SRM_SSRM6_2-Holly</t>
-  </si>
-  <si>
-    <t>Weapon_SRM_SSRM6_1-Irian</t>
-  </si>
-  <si>
-    <t>Weapon_SRM_SSRM6_1-Holly</t>
-  </si>
-  <si>
-    <t>Weapon_SRM_SSRM6_0-STOCK</t>
-  </si>
-  <si>
-    <t>Weapon_SRM_SSRM4_3-Valiant</t>
-  </si>
-  <si>
-    <t>Weapon_SRM_SSRM4_2-Valiant</t>
-  </si>
-  <si>
-    <t>Weapon_SRM_SSRM4_2-Irian</t>
-  </si>
-  <si>
-    <t>Weapon_SRM_SSRM4_2-Holly</t>
-  </si>
-  <si>
-    <t>Weapon_SRM_SSRM4_1-Irian</t>
-  </si>
-  <si>
-    <t>Weapon_SRM_SSRM4_1-Holly</t>
-  </si>
-  <si>
-    <t>Weapon_SRM_SSRM4_0-STOCK</t>
-  </si>
-  <si>
-    <t>Weapon_SRM_SSRM2_3-Valiant</t>
-  </si>
-  <si>
-    <t>Weapon_SRM_SSRM2_2-Valiant</t>
-  </si>
-  <si>
-    <t>Weapon_SRM_SSRM2_2-Irian</t>
-  </si>
-  <si>
-    <t>Weapon_SRM_SSRM2_2-Holly</t>
-  </si>
-  <si>
-    <t>Weapon_SRM_SSRM2_1-Irian</t>
-  </si>
-  <si>
-    <t>Weapon_SRM_SSRM2_1-Holly</t>
-  </si>
-  <si>
-    <t>Weapon_SRM_SSRM2_0-STOCK</t>
-  </si>
-  <si>
-    <t>Weapon_SRM_SRM6_3-Lockheed</t>
-  </si>
-  <si>
-    <t>Weapon_SRM_SRM6_3-Irian</t>
-  </si>
-  <si>
-    <t>Weapon_SRM_SRM6_3-Holly</t>
-  </si>
-  <si>
-    <t>Weapon_SRM_SRM6_3-Harvester</t>
-  </si>
-  <si>
-    <t>Weapon_SRM_SRM6_3-Coventry</t>
-  </si>
-  <si>
-    <t>Weapon_SRM_SRM6_2-Lockheed</t>
-  </si>
-  <si>
-    <t>Weapon_SRM_SRM6_2-Harvester</t>
-  </si>
-  <si>
-    <t>Weapon_SRM_SRM6_2-Coventry</t>
-  </si>
-  <si>
-    <t>Weapon_SRM_SRM6_1-Valiant</t>
-  </si>
-  <si>
-    <t>Weapon_SRM_SRM6_1-Lockheed</t>
-  </si>
-  <si>
-    <t>Weapon_SRM_SRM6_1-Harvester</t>
-  </si>
-  <si>
-    <t>Weapon_SRM_SRM6_1-Coventry</t>
-  </si>
-  <si>
-    <t>Weapon_SRM_SRM4_3-Lockheed</t>
-  </si>
-  <si>
-    <t>Weapon_SRM_SRM4_3-Irian</t>
-  </si>
-  <si>
-    <t>Weapon_SRM_SRM4_3-Holly</t>
-  </si>
-  <si>
-    <t>Weapon_SRM_SRM4_3-Harvester</t>
-  </si>
-  <si>
-    <t>Weapon_SRM_SRM4_3-Coventry</t>
-  </si>
-  <si>
-    <t>Weapon_SRM_SRM4_2-Lockheed</t>
-  </si>
-  <si>
-    <t>Weapon_SRM_SRM4_2-Harvester</t>
-  </si>
-  <si>
-    <t>Weapon_SRM_SRM4_2-Coventry</t>
-  </si>
-  <si>
-    <t>Weapon_SRM_SRM4_1-Valiant</t>
-  </si>
-  <si>
-    <t>Weapon_SRM_SRM4_1-Lockheed</t>
-  </si>
-  <si>
-    <t>Weapon_SRM_SRM4_1-Harvester</t>
-  </si>
-  <si>
-    <t>Weapon_SRM_SRM4_1-Coventry</t>
-  </si>
-  <si>
-    <t>Weapon_SRM_SRM2_3-Lockheed</t>
-  </si>
-  <si>
-    <t>Weapon_SRM_SRM2_3-Irian</t>
-  </si>
-  <si>
-    <t>Weapon_SRM_SRM2_3-Holly</t>
-  </si>
-  <si>
-    <t>Weapon_SRM_SRM2_3-Harvester</t>
-  </si>
-  <si>
-    <t>Weapon_SRM_SRM2_3-Coventry</t>
-  </si>
-  <si>
-    <t>Weapon_SRM_SRM2_2-Lockheed</t>
-  </si>
-  <si>
-    <t>Weapon_SRM_SRM2_2-Harvester</t>
-  </si>
-  <si>
-    <t>Weapon_SRM_SRM2_2-Coventry</t>
-  </si>
-  <si>
-    <t>Weapon_SRM_SRM2_1-Valiant</t>
-  </si>
-  <si>
-    <t>Weapon_SRM_SRM2_1-Lockheed</t>
-  </si>
-  <si>
-    <t>Weapon_SRM_SRM2_1-Harvester</t>
-  </si>
-  <si>
-    <t>Weapon_SRM_SRM2_1-Coventry</t>
-  </si>
-  <si>
-    <t>Weapon_PPC_PPCSnub_2-Magna</t>
-  </si>
-  <si>
-    <t>Weapon_PPC_PPCSnub_2-Donal</t>
-  </si>
-  <si>
-    <t>Weapon_PPC_PPCSnub_2-Ceres_Arms</t>
-  </si>
-  <si>
-    <t>Weapon_PPC_PPCSnub_1-Magna</t>
-  </si>
-  <si>
-    <t>Weapon_PPC_PPCSnub_1-Donal</t>
-  </si>
-  <si>
-    <t>Weapon_PPC_PPCSnub_1-Ceres_Arms</t>
-  </si>
-  <si>
-    <t>Weapon_Narc_Standard_2-Kali_Yama</t>
-  </si>
-  <si>
-    <t>Weapon_Narc_Standard_1-Ceres_Arms</t>
-  </si>
-  <si>
-    <t>Weapon_Narc_Standard_0-STOCK</t>
-  </si>
-  <si>
-    <t>Weapon_MachineGun_TwinMachineGun_2-Brigadier</t>
-  </si>
-  <si>
-    <t>Weapon_MachineGun_TwinMachineGun_1-VMI</t>
-  </si>
-  <si>
-    <t>Weapon_MachineGun_TwinMachineGun_0-STOCK</t>
-  </si>
-  <si>
-    <t>Weapon_LRM_LRM5_3-Telos</t>
-  </si>
-  <si>
-    <t>Weapon_LRM_LRM5_3-Drago</t>
-  </si>
-  <si>
-    <t>Weapon_LRM_LRM5_3-Delta</t>
-  </si>
-  <si>
-    <t>Weapon_LRM_LRM5_3-Coventry</t>
-  </si>
-  <si>
-    <t>Weapon_LRM_LRM5_3-Concordat</t>
-  </si>
-  <si>
-    <t>Weapon_LRM_LRM5_2-Drago</t>
-  </si>
-  <si>
-    <t>Weapon_LRM_LRM5_2-Coventry</t>
-  </si>
-  <si>
-    <t>Weapon_LRM_LRM5_2-Concordat</t>
-  </si>
-  <si>
-    <t>Weapon_LRM_LRM5_1-Zeus</t>
-  </si>
-  <si>
-    <t>Weapon_LRM_LRM5_1-Drago</t>
-  </si>
-  <si>
-    <t>Weapon_LRM_LRM5_1-Coventry</t>
-  </si>
-  <si>
-    <t>Weapon_LRM_LRM5_1-Concordat</t>
-  </si>
-  <si>
-    <t>Weapon_LRM_LRM20_3-Telos</t>
-  </si>
-  <si>
-    <t>Weapon_LRM_LRM20_3-Drago</t>
-  </si>
-  <si>
-    <t>Weapon_LRM_LRM20_3-Delta</t>
-  </si>
-  <si>
-    <t>Weapon_LRM_LRM20_3-Coventry</t>
-  </si>
-  <si>
-    <t>Weapon_LRM_LRM20_3-Concordat</t>
-  </si>
-  <si>
-    <t>Weapon_LRM_LRM20_2-Drago</t>
-  </si>
-  <si>
-    <t>Weapon_LRM_LRM20_2-Coventry</t>
-  </si>
-  <si>
-    <t>Weapon_LRM_LRM20_2-Concordat</t>
-  </si>
-  <si>
-    <t>Weapon_LRM_LRM20_1-Zeus</t>
-  </si>
-  <si>
-    <t>Weapon_LRM_LRM20_1-Drago</t>
-  </si>
-  <si>
-    <t>Weapon_LRM_LRM20_1-Coventry</t>
-  </si>
-  <si>
-    <t>Weapon_LRM_LRM20_1-Concordat</t>
-  </si>
-  <si>
-    <t>Weapon_LRM_LRM15_3-Telos</t>
-  </si>
-  <si>
-    <t>Weapon_LRM_LRM15_3-Drago</t>
-  </si>
-  <si>
-    <t>Weapon_LRM_LRM15_3-Delta</t>
-  </si>
-  <si>
-    <t>Weapon_LRM_LRM15_3-Coventry</t>
-  </si>
-  <si>
-    <t>Weapon_LRM_LRM15_3-Concordat</t>
-  </si>
-  <si>
-    <t>Weapon_LRM_LRM15_2-Drago</t>
-  </si>
-  <si>
-    <t>Weapon_LRM_LRM15_2-Coventry</t>
-  </si>
-  <si>
-    <t>Weapon_LRM_LRM15_2-Concordat</t>
-  </si>
-  <si>
-    <t>Weapon_LRM_LRM15_1-Zeus</t>
-  </si>
-  <si>
-    <t>Weapon_LRM_LRM15_1-Drago</t>
-  </si>
-  <si>
-    <t>Weapon_LRM_LRM15_1-Coventry</t>
-  </si>
-  <si>
-    <t>Weapon_LRM_LRM15_1-Concordat</t>
-  </si>
-  <si>
-    <t>Weapon_LRM_LRM10_3-Telos</t>
-  </si>
-  <si>
-    <t>Weapon_LRM_LRM10_3-Drago</t>
-  </si>
-  <si>
-    <t>Weapon_LRM_LRM10_3-Delta</t>
-  </si>
-  <si>
-    <t>Weapon_LRM_LRM10_3-Coventry</t>
-  </si>
-  <si>
-    <t>Weapon_LRM_LRM10_3-Concordat</t>
-  </si>
-  <si>
-    <t>Weapon_LRM_LRM10_2-Drago</t>
-  </si>
-  <si>
-    <t>Weapon_LRM_LRM10_2-Coventry</t>
-  </si>
-  <si>
-    <t>Weapon_LRM_LRM10_2-Concordat</t>
-  </si>
-  <si>
-    <t>Weapon_LRM_LRM10_1-Zeus</t>
-  </si>
-  <si>
-    <t>Weapon_LRM_LRM10_1-Drago</t>
-  </si>
-  <si>
-    <t>Weapon_LRM_LRM10_1-Coventry</t>
-  </si>
-  <si>
-    <t>Weapon_LRM_LRM10_1-Concordat</t>
-  </si>
-  <si>
-    <t>Weapon_Autocannon_UAC5_2-Mydron</t>
-  </si>
-  <si>
-    <t>Weapon_Autocannon_UAC5_1-Mydron</t>
-  </si>
-  <si>
-    <t>Weapon_Autocannon_UAC5_0-STOCK</t>
-  </si>
-  <si>
-    <t>Weapon_Autocannon_UAC2_2-Imperator</t>
-  </si>
-  <si>
-    <t>Weapon_Autocannon_UAC2_1-Imperator</t>
-  </si>
-  <si>
-    <t>Weapon_Autocannon_UAC2_0-STOCK</t>
-  </si>
-  <si>
-    <t>Weapon_Autocannon_UAC10_2-Federated</t>
-  </si>
-  <si>
-    <t>Weapon_Autocannon_UAC10_1-Federated</t>
-  </si>
-  <si>
-    <t>Weapon_Autocannon_UAC10_0-STOCK</t>
-  </si>
-  <si>
-    <t>Weapon_Autocannon_LB5X_2-GM</t>
-  </si>
-  <si>
-    <t>Weapon_Autocannon_LB5X_1-GM</t>
-  </si>
-  <si>
-    <t>Weapon_Autocannon_LB5X_0-STOCK</t>
-  </si>
-  <si>
-    <t>Weapon_Autocannon_LB2X_2-Defiance</t>
-  </si>
-  <si>
-    <t>Weapon_Autocannon_LB2X_1-Defiance</t>
-  </si>
-  <si>
-    <t>Weapon_Autocannon_LB2X_0-STOCK</t>
-  </si>
-  <si>
-    <t>Weapon_Autocannon_LB20X_2-Shengli_Arms</t>
-  </si>
-  <si>
-    <t>Weapon_Autocannon_LB20X_2-Imperator</t>
-  </si>
-  <si>
-    <t>Weapon_Autocannon_LB20X_1-Shengli_Arms</t>
-  </si>
-  <si>
-    <t>Weapon_Autocannon_LB20X_0-STOCK</t>
-  </si>
-  <si>
-    <t>Weapon_Autocannon_LB10X_2-Western</t>
-  </si>
-  <si>
-    <t>Weapon_Autocannon_LB10X_1-Western</t>
-  </si>
-  <si>
-    <t>Weapon_Autocannon_LB10X_0-STOCK</t>
-  </si>
-  <si>
-    <t>Weapon_Autocannon_AC5_3-ZeusBolt</t>
-  </si>
-  <si>
-    <t>Weapon_Autocannon_AC5_3-Kali_Yama</t>
-  </si>
-  <si>
-    <t>Weapon_Autocannon_AC5_3-Imperator</t>
-  </si>
-  <si>
-    <t>Weapon_Autocannon_AC5_3-Federated</t>
-  </si>
-  <si>
-    <t>Weapon_Autocannon_AC5_3-Defiance</t>
-  </si>
-  <si>
-    <t>Weapon_Autocannon_AC5_2-ZeusBolt</t>
-  </si>
-  <si>
-    <t>Weapon_Autocannon_AC5_1-ZeusBolt</t>
-  </si>
-  <si>
-    <t>Weapon_Autocannon_AC5_1-Mydron</t>
-  </si>
-  <si>
-    <t>Weapon_Autocannon_AC2_3-ZeusBolt</t>
-  </si>
-  <si>
-    <t>Weapon_Autocannon_AC2_3-Mydron</t>
-  </si>
-  <si>
-    <t>Weapon_Autocannon_AC2_3-Kali_Yama</t>
-  </si>
-  <si>
-    <t>Weapon_Autocannon_AC2_3-Federated</t>
-  </si>
-  <si>
-    <t>Weapon_Autocannon_AC2_3-Defiance</t>
-  </si>
-  <si>
-    <t>Weapon_Autocannon_AC2_2-ZeusBolt</t>
-  </si>
-  <si>
-    <t>Weapon_Autocannon_AC2_1-ZeusBolt</t>
-  </si>
-  <si>
-    <t>Weapon_Autocannon_AC2_1-Imperator</t>
-  </si>
-  <si>
-    <t>Weapon_Autocannon_AC10_3-ZeusBolt</t>
-  </si>
-  <si>
-    <t>Weapon_Autocannon_AC10_3-Mydron</t>
-  </si>
-  <si>
-    <t>Weapon_Autocannon_AC10_3-Kali_Yama</t>
-  </si>
-  <si>
-    <t>Weapon_Autocannon_AC10_3-Imperator</t>
-  </si>
-  <si>
-    <t>Weapon_Autocannon_AC10_3-Defiance</t>
-  </si>
-  <si>
-    <t>Weapon_Autocannon_AC10_2-ZeusBolt</t>
-  </si>
-  <si>
-    <t>Weapon_Autocannon_AC10_1-ZeusBolt</t>
-  </si>
-  <si>
-    <t>Weapon_Autocannon_AC10_1-Federated</t>
-  </si>
-  <si>
-    <t>Weapon_AMS_2</t>
-  </si>
-  <si>
-    <t>Weapon_AMS_1</t>
-  </si>
-  <si>
-    <t>Weapon_AMS</t>
-  </si>
-  <si>
-    <t>Weapon_MachineGun_MachineGun_2-VMI</t>
-  </si>
-  <si>
-    <t>Weapon_MachineGun_MachineGun_2-Brigadier</t>
-  </si>
-  <si>
-    <t>Weapon_MachineGun_MachineGun_1-VMI</t>
-  </si>
-  <si>
-    <t>Weapon_MachineGun_MachineGun_1-Brigadier</t>
-  </si>
-  <si>
-    <t>Weapon_Gauss_Gauss_2-M9</t>
-  </si>
-  <si>
-    <t>Weapon_Gauss_Gauss_1-M7</t>
-  </si>
-  <si>
-    <t>Weapon_SRM_SRM6_3-Valiant</t>
-  </si>
-  <si>
-    <t>Weapon_SRM_SRM6_2-Valiant</t>
-  </si>
-  <si>
-    <t>Weapon_SRM_SRM6_2-Irian</t>
-  </si>
-  <si>
-    <t>Weapon_SRM_SRM6_2-Holly</t>
-  </si>
-  <si>
-    <t>Weapon_SRM_SRM6_1-Irian</t>
-  </si>
-  <si>
-    <t>Weapon_SRM_SRM6_1-Holly</t>
-  </si>
-  <si>
-    <t>Weapon_SRM_SRM6_0-STOCK</t>
-  </si>
-  <si>
-    <t>Weapon_SRM_SRM4_3-Valiant</t>
-  </si>
-  <si>
-    <t>Weapon_SRM_SRM4_2-Valiant</t>
-  </si>
-  <si>
-    <t>Weapon_SRM_SRM4_2-Irian</t>
-  </si>
-  <si>
-    <t>Weapon_SRM_SRM4_2-Holly</t>
-  </si>
-  <si>
-    <t>Weapon_SRM_SRM4_1-Irian</t>
-  </si>
-  <si>
-    <t>Weapon_SRM_SRM4_1-Holly</t>
-  </si>
-  <si>
-    <t>Weapon_SRM_SRM4_0-STOCK</t>
-  </si>
-  <si>
-    <t>Weapon_SRM_SRM2_3-Valiant</t>
-  </si>
-  <si>
-    <t>Weapon_SRM_SRM2_2-Valiant</t>
-  </si>
-  <si>
-    <t>Weapon_SRM_SRM2_2-Irian</t>
-  </si>
-  <si>
-    <t>Weapon_SRM_SRM2_2-Holly</t>
-  </si>
-  <si>
-    <t>Weapon_SRM_SRM2_1-Irian</t>
-  </si>
-  <si>
-    <t>Weapon_SRM_SRM2_1-Holly</t>
-  </si>
-  <si>
-    <t>Weapon_MachineGun_MachineGun_0-STOCK</t>
-  </si>
-  <si>
-    <t>Weapon_LRM_LRM5_3-Zeus</t>
-  </si>
-  <si>
-    <t>Weapon_LRM_LRM5_2-Zeus</t>
-  </si>
-  <si>
-    <t>Weapon_LRM_LRM5_2-Telos</t>
-  </si>
-  <si>
-    <t>Weapon_LRM_LRM5_2-LongFire</t>
-  </si>
-  <si>
-    <t>Weapon_LRM_LRM5_2-Delta</t>
-  </si>
-  <si>
-    <t>Weapon_LRM_LRM5_1-Telos</t>
-  </si>
-  <si>
-    <t>Weapon_LRM_LRM5_1-LongFire</t>
-  </si>
-  <si>
-    <t>Weapon_LRM_LRM5_1-Delta</t>
-  </si>
-  <si>
-    <t>Weapon_LRM_LRM20_3-Zeus</t>
-  </si>
-  <si>
-    <t>Weapon_LRM_LRM20_2-Zeus</t>
-  </si>
-  <si>
-    <t>Weapon_LRM_LRM20_2-Telos</t>
-  </si>
-  <si>
-    <t>Weapon_LRM_LRM20_2-LongFire</t>
-  </si>
-  <si>
-    <t>Weapon_LRM_LRM20_2-Delta</t>
-  </si>
-  <si>
-    <t>Weapon_LRM_LRM20_1-Telos</t>
-  </si>
-  <si>
-    <t>Weapon_LRM_LRM20_1-LongFire</t>
-  </si>
-  <si>
-    <t>Weapon_LRM_LRM20_1-Delta</t>
-  </si>
-  <si>
-    <t>Weapon_LRM_LRM20_0-STOCK</t>
-  </si>
-  <si>
-    <t>Weapon_LRM_LRM15_3-Zeus</t>
-  </si>
-  <si>
-    <t>Weapon_LRM_LRM15_2-Zeus</t>
-  </si>
-  <si>
-    <t>Weapon_LRM_LRM15_2-Telos</t>
-  </si>
-  <si>
-    <t>Weapon_LRM_LRM15_2-LongFire</t>
-  </si>
-  <si>
-    <t>Weapon_LRM_LRM15_2-Delta</t>
-  </si>
-  <si>
-    <t>Weapon_LRM_LRM15_1-Telos</t>
-  </si>
-  <si>
-    <t>Weapon_LRM_LRM15_1-LongFire</t>
-  </si>
-  <si>
-    <t>Weapon_LRM_LRM15_1-Delta</t>
-  </si>
-  <si>
-    <t>Weapon_LRM_LRM15_0-STOCK</t>
-  </si>
-  <si>
-    <t>Weapon_LRM_LRM10_3-Zeus</t>
-  </si>
-  <si>
-    <t>Weapon_LRM_LRM10_2-Zeus</t>
-  </si>
-  <si>
-    <t>Weapon_LRM_LRM10_2-Telos</t>
-  </si>
-  <si>
-    <t>Weapon_LRM_LRM10_2-LongFire</t>
-  </si>
-  <si>
-    <t>Weapon_LRM_LRM10_2-Delta</t>
-  </si>
-  <si>
-    <t>Weapon_LRM_LRM10_1-Telos</t>
-  </si>
-  <si>
-    <t>Weapon_LRM_LRM10_1-LongFire</t>
-  </si>
-  <si>
-    <t>Weapon_LRM_LRM10_1-Delta</t>
-  </si>
-  <si>
-    <t>Weapon_LRM_LRM10_0-STOCK</t>
-  </si>
-  <si>
-    <t>Weapon_Gauss_Gauss_0-STOCK</t>
-  </si>
-  <si>
-    <t>Weapon_Autocannon_AC5_3-Mydron</t>
-  </si>
-  <si>
-    <t>Weapon_Autocannon_AC5_2-Mydron</t>
-  </si>
-  <si>
-    <t>Weapon_Autocannon_AC5_2-Kali_Yama</t>
-  </si>
-  <si>
-    <t>Weapon_Autocannon_AC5_2-Imperator</t>
-  </si>
-  <si>
-    <t>Weapon_Autocannon_AC5_2-Federated</t>
-  </si>
-  <si>
-    <t>Weapon_Autocannon_AC5_2-Defiance</t>
-  </si>
-  <si>
-    <t>Weapon_Autocannon_AC5_1-Kali_Yama</t>
-  </si>
-  <si>
-    <t>Weapon_Autocannon_AC5_1-Imperator</t>
-  </si>
-  <si>
-    <t>Weapon_Autocannon_AC5_1-Federated</t>
-  </si>
-  <si>
-    <t>Weapon_Autocannon_AC5_1-Defiance</t>
-  </si>
-  <si>
-    <t>Weapon_Autocannon_AC2_3-Imperator</t>
-  </si>
-  <si>
-    <t>Weapon_Autocannon_AC2_2-Mydron</t>
-  </si>
-  <si>
-    <t>Weapon_Autocannon_AC2_2-Kali_Yama</t>
-  </si>
-  <si>
-    <t>Weapon_Autocannon_AC2_2-Imperator</t>
-  </si>
-  <si>
-    <t>Weapon_Autocannon_AC2_2-Federated</t>
-  </si>
-  <si>
-    <t>Weapon_Autocannon_AC2_2-Defiance</t>
-  </si>
-  <si>
-    <t>Weapon_Autocannon_AC2_1-Mydron</t>
-  </si>
-  <si>
-    <t>Weapon_Autocannon_AC2_1-Kali_Yama</t>
-  </si>
-  <si>
-    <t>Weapon_Autocannon_AC2_1-Federated</t>
-  </si>
-  <si>
-    <t>Weapon_Autocannon_AC2_1-Defiance</t>
-  </si>
-  <si>
-    <t>Weapon_Autocannon_AC2_0-STOCK</t>
-  </si>
-  <si>
-    <t>Weapon_Autocannon_AC10_3-Federated</t>
-  </si>
-  <si>
-    <t>Weapon_Autocannon_AC10_2-Mydron</t>
-  </si>
-  <si>
-    <t>Weapon_Autocannon_AC10_2-Kali_Yama</t>
-  </si>
-  <si>
-    <t>Weapon_Autocannon_AC10_2-Imperator</t>
-  </si>
-  <si>
-    <t>Weapon_Autocannon_AC10_2-Federated</t>
-  </si>
-  <si>
-    <t>Weapon_Autocannon_AC10_2-Defiance</t>
-  </si>
-  <si>
-    <t>Weapon_Autocannon_AC10_1-Mydron</t>
-  </si>
-  <si>
-    <t>Weapon_Autocannon_AC10_1-Kali_Yama</t>
-  </si>
-  <si>
-    <t>Weapon_Autocannon_AC10_1-Imperator</t>
-  </si>
-  <si>
-    <t>Weapon_Autocannon_AC10_1-Defiance</t>
-  </si>
-  <si>
-    <t>Weapon_Autocannon_AC10_0-STOCK</t>
   </si>
   <si>
     <t>Weapon_Autocannon_UAC20_2-Kali_Yama</t>
@@ -10653,7 +10653,7 @@
         <v>0</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>443</v>
+        <v>355</v>
       </c>
     </row>
     <row r="6">
@@ -10661,7 +10661,7 @@
         <v>776</v>
       </c>
       <c r="B6" s="0" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>670</v>
@@ -10672,10 +10672,10 @@
         <v>777</v>
       </c>
       <c r="B7" s="0" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>355</v>
+        <v>670</v>
       </c>
     </row>
     <row r="8">
@@ -10683,7 +10683,7 @@
         <v>778</v>
       </c>
       <c r="B8" s="0" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>670</v>
@@ -10719,7 +10719,7 @@
         <v>0</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>670</v>
+        <v>443</v>
       </c>
     </row>
     <row r="12">
@@ -10738,7 +10738,7 @@
         <v>783</v>
       </c>
       <c r="B13" s="0" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>670</v>
@@ -10749,7 +10749,7 @@
         <v>784</v>
       </c>
       <c r="B14" s="0" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>670</v>
@@ -10760,7 +10760,7 @@
         <v>785</v>
       </c>
       <c r="B15" s="0" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>670</v>
@@ -14033,10 +14033,10 @@
         <v>1073</v>
       </c>
       <c r="B2" s="0" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>588</v>
+        <v>698</v>
       </c>
     </row>
     <row r="3">
@@ -14286,10 +14286,10 @@
         <v>1094</v>
       </c>
       <c r="B25" s="0" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>431</v>
+        <v>698</v>
       </c>
     </row>
     <row r="26">
@@ -14297,10 +14297,10 @@
         <v>1095</v>
       </c>
       <c r="B26" s="0" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>155</v>
+        <v>698</v>
       </c>
     </row>
     <row r="27">
@@ -14311,7 +14311,7 @@
         <v>1</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>147</v>
+        <v>431</v>
       </c>
     </row>
     <row r="28">
@@ -14322,7 +14322,7 @@
         <v>1</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>58</v>
+        <v>155</v>
       </c>
     </row>
     <row r="29">
@@ -14333,7 +14333,7 @@
         <v>1</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>454</v>
+        <v>147</v>
       </c>
     </row>
     <row r="30">
@@ -14341,10 +14341,10 @@
         <v>1099</v>
       </c>
       <c r="B30" s="0" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>698</v>
+        <v>58</v>
       </c>
     </row>
     <row r="31">
@@ -14352,10 +14352,10 @@
         <v>1100</v>
       </c>
       <c r="B31" s="0" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>698</v>
+        <v>454</v>
       </c>
     </row>
     <row r="32">
@@ -14366,7 +14366,7 @@
         <v>1</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>670</v>
+        <v>588</v>
       </c>
     </row>
     <row r="33">
@@ -14509,7 +14509,7 @@
         <v>1</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>698</v>
+        <v>491</v>
       </c>
     </row>
     <row r="46">
@@ -14542,7 +14542,7 @@
         <v>1</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>363</v>
+        <v>698</v>
       </c>
     </row>
     <row r="49">
@@ -14553,7 +14553,7 @@
         <v>1</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>52</v>
+        <v>698</v>
       </c>
     </row>
     <row r="50">
@@ -14564,7 +14564,7 @@
         <v>1</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>149</v>
+        <v>698</v>
       </c>
     </row>
     <row r="51">
@@ -14605,7 +14605,7 @@
         <v>1123</v>
       </c>
       <c r="B54" s="0" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C54" s="0" t="s">
         <v>698</v>
@@ -14679,7 +14679,7 @@
     </row>
     <row r="61">
       <c r="A61" s="0" t="s">
-        <v>1109</v>
+        <v>1130</v>
       </c>
       <c r="B61" s="0" t="b">
         <v>1</v>
@@ -14690,7 +14690,7 @@
     </row>
     <row r="62">
       <c r="A62" s="0" t="s">
-        <v>1130</v>
+        <v>1131</v>
       </c>
       <c r="B62" s="0" t="b">
         <v>1</v>
@@ -14701,43 +14701,43 @@
     </row>
     <row r="63">
       <c r="A63" s="0" t="s">
-        <v>1131</v>
+        <v>1132</v>
       </c>
       <c r="B63" s="0" t="b">
         <v>1</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>188</v>
+        <v>698</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="0" t="s">
-        <v>1113</v>
+        <v>1133</v>
       </c>
       <c r="B64" s="0" t="b">
         <v>1</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>698</v>
+        <v>363</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="0" t="s">
-        <v>1132</v>
+        <v>1134</v>
       </c>
       <c r="B65" s="0" t="b">
         <v>1</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>698</v>
+        <v>52</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="0" t="s">
-        <v>1133</v>
+        <v>1135</v>
       </c>
       <c r="B66" s="0" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C66" s="0" t="s">
         <v>698</v>
@@ -14745,51 +14745,51 @@
     </row>
     <row r="67">
       <c r="A67" s="0" t="s">
-        <v>1134</v>
+        <v>1136</v>
       </c>
       <c r="B67" s="0" t="b">
         <v>1</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>52</v>
+        <v>698</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="0" t="s">
-        <v>1135</v>
+        <v>1137</v>
       </c>
       <c r="B68" s="0" t="b">
         <v>1</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>698</v>
+        <v>462</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="0" t="s">
-        <v>1136</v>
+        <v>1138</v>
       </c>
       <c r="B69" s="0" t="b">
         <v>1</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>95</v>
+        <v>698</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="0" t="s">
-        <v>1137</v>
+        <v>1139</v>
       </c>
       <c r="B70" s="0" t="b">
         <v>1</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>470</v>
+        <v>149</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="0" t="s">
-        <v>1138</v>
+        <v>1140</v>
       </c>
       <c r="B71" s="0" t="b">
         <v>1</v>
@@ -14800,10 +14800,10 @@
     </row>
     <row r="72">
       <c r="A72" s="0" t="s">
-        <v>1139</v>
+        <v>1141</v>
       </c>
       <c r="B72" s="0" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C72" s="0" t="s">
         <v>698</v>
@@ -14811,7 +14811,7 @@
     </row>
     <row r="73">
       <c r="A73" s="0" t="s">
-        <v>1140</v>
+        <v>1142</v>
       </c>
       <c r="B73" s="0" t="b">
         <v>1</v>
@@ -14822,10 +14822,10 @@
     </row>
     <row r="74">
       <c r="A74" s="0" t="s">
-        <v>1141</v>
+        <v>1143</v>
       </c>
       <c r="B74" s="0" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C74" s="0" t="s">
         <v>698</v>
@@ -14833,7 +14833,7 @@
     </row>
     <row r="75">
       <c r="A75" s="0" t="s">
-        <v>1142</v>
+        <v>1144</v>
       </c>
       <c r="B75" s="0" t="b">
         <v>1</v>
@@ -14844,7 +14844,7 @@
     </row>
     <row r="76">
       <c r="A76" s="0" t="s">
-        <v>1143</v>
+        <v>1145</v>
       </c>
       <c r="B76" s="0" t="b">
         <v>1</v>
@@ -14855,7 +14855,7 @@
     </row>
     <row r="77">
       <c r="A77" s="0" t="s">
-        <v>1144</v>
+        <v>1146</v>
       </c>
       <c r="B77" s="0" t="b">
         <v>1</v>
@@ -14866,18 +14866,18 @@
     </row>
     <row r="78">
       <c r="A78" s="0" t="s">
-        <v>1145</v>
+        <v>1147</v>
       </c>
       <c r="B78" s="0" t="b">
         <v>1</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>698</v>
+        <v>95</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="0" t="s">
-        <v>1146</v>
+        <v>1148</v>
       </c>
       <c r="B79" s="0" t="b">
         <v>1</v>
@@ -14888,18 +14888,18 @@
     </row>
     <row r="80">
       <c r="A80" s="0" t="s">
-        <v>1147</v>
+        <v>1149</v>
       </c>
       <c r="B80" s="0" t="b">
         <v>1</v>
       </c>
       <c r="C80" s="0" t="s">
-        <v>698</v>
+        <v>153</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="0" t="s">
-        <v>1148</v>
+        <v>1150</v>
       </c>
       <c r="B81" s="0" t="b">
         <v>1</v>
@@ -14910,7 +14910,7 @@
     </row>
     <row r="82">
       <c r="A82" s="0" t="s">
-        <v>1149</v>
+        <v>1113</v>
       </c>
       <c r="B82" s="0" t="b">
         <v>1</v>
@@ -14921,7 +14921,7 @@
     </row>
     <row r="83">
       <c r="A83" s="0" t="s">
-        <v>1150</v>
+        <v>1151</v>
       </c>
       <c r="B83" s="0" t="b">
         <v>1</v>
@@ -14932,7 +14932,7 @@
     </row>
     <row r="84">
       <c r="A84" s="0" t="s">
-        <v>1151</v>
+        <v>1152</v>
       </c>
       <c r="B84" s="0" t="b">
         <v>1</v>
@@ -14943,13 +14943,13 @@
     </row>
     <row r="85">
       <c r="A85" s="0" t="s">
-        <v>1152</v>
+        <v>1117</v>
       </c>
       <c r="B85" s="0" t="b">
         <v>1</v>
       </c>
       <c r="C85" s="0" t="s">
-        <v>491</v>
+        <v>698</v>
       </c>
     </row>
     <row r="86">
@@ -14971,7 +14971,7 @@
         <v>1</v>
       </c>
       <c r="C87" s="0" t="s">
-        <v>698</v>
+        <v>37</v>
       </c>
     </row>
     <row r="88">
@@ -14982,7 +14982,7 @@
         <v>1</v>
       </c>
       <c r="C88" s="0" t="s">
-        <v>698</v>
+        <v>457</v>
       </c>
     </row>
     <row r="89">
@@ -14993,7 +14993,7 @@
         <v>1</v>
       </c>
       <c r="C89" s="0" t="s">
-        <v>52</v>
+        <v>346</v>
       </c>
     </row>
     <row r="90">
@@ -15001,7 +15001,7 @@
         <v>1157</v>
       </c>
       <c r="B90" s="0" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C90" s="0" t="s">
         <v>698</v>
@@ -15015,7 +15015,7 @@
         <v>1</v>
       </c>
       <c r="C91" s="0" t="s">
-        <v>153</v>
+        <v>698</v>
       </c>
     </row>
     <row r="92">
@@ -15031,7 +15031,7 @@
     </row>
     <row r="93">
       <c r="A93" s="0" t="s">
-        <v>1160</v>
+        <v>1125</v>
       </c>
       <c r="B93" s="0" t="b">
         <v>1</v>
@@ -15042,7 +15042,7 @@
     </row>
     <row r="94">
       <c r="A94" s="0" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="B94" s="0" t="b">
         <v>1</v>
@@ -15053,18 +15053,18 @@
     </row>
     <row r="95">
       <c r="A95" s="0" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="B95" s="0" t="b">
         <v>1</v>
       </c>
       <c r="C95" s="0" t="s">
-        <v>462</v>
+        <v>188</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="0" t="s">
-        <v>1163</v>
+        <v>1129</v>
       </c>
       <c r="B96" s="0" t="b">
         <v>1</v>
@@ -15075,10 +15075,10 @@
     </row>
     <row r="97">
       <c r="A97" s="0" t="s">
-        <v>1164</v>
+        <v>1162</v>
       </c>
       <c r="B97" s="0" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C97" s="0" t="s">
         <v>698</v>
@@ -15086,10 +15086,10 @@
     </row>
     <row r="98">
       <c r="A98" s="0" t="s">
-        <v>1165</v>
+        <v>1163</v>
       </c>
       <c r="B98" s="0" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C98" s="0" t="s">
         <v>698</v>
@@ -15097,7 +15097,7 @@
     </row>
     <row r="99">
       <c r="A99" s="0" t="s">
-        <v>1166</v>
+        <v>1164</v>
       </c>
       <c r="B99" s="0" t="b">
         <v>1</v>
@@ -15108,51 +15108,51 @@
     </row>
     <row r="100">
       <c r="A100" s="0" t="s">
-        <v>1167</v>
+        <v>1165</v>
       </c>
       <c r="B100" s="0" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C100" s="0" t="s">
-        <v>698</v>
+        <v>526</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="0" t="s">
-        <v>1168</v>
+        <v>1166</v>
       </c>
       <c r="B101" s="0" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C101" s="0" t="s">
-        <v>698</v>
+        <v>670</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="0" t="s">
-        <v>1169</v>
+        <v>1167</v>
       </c>
       <c r="B102" s="0" t="b">
         <v>1</v>
       </c>
       <c r="C102" s="0" t="s">
-        <v>288</v>
+        <v>698</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="0" t="s">
-        <v>1170</v>
+        <v>1168</v>
       </c>
       <c r="B103" s="0" t="b">
         <v>1</v>
       </c>
       <c r="C103" s="0" t="s">
-        <v>37</v>
+        <v>698</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="0" t="s">
-        <v>1171</v>
+        <v>1169</v>
       </c>
       <c r="B104" s="0" t="b">
         <v>1</v>
@@ -15163,18 +15163,18 @@
     </row>
     <row r="105">
       <c r="A105" s="0" t="s">
-        <v>1172</v>
+        <v>1170</v>
       </c>
       <c r="B105" s="0" t="b">
         <v>1</v>
       </c>
       <c r="C105" s="0" t="s">
-        <v>153</v>
+        <v>698</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="0" t="s">
-        <v>1173</v>
+        <v>1171</v>
       </c>
       <c r="B106" s="0" t="b">
         <v>1</v>
@@ -15185,7 +15185,7 @@
     </row>
     <row r="107">
       <c r="A107" s="0" t="s">
-        <v>1151</v>
+        <v>1172</v>
       </c>
       <c r="B107" s="0" t="b">
         <v>1</v>
@@ -15196,18 +15196,18 @@
     </row>
     <row r="108">
       <c r="A108" s="0" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
       <c r="B108" s="0" t="b">
         <v>1</v>
       </c>
       <c r="C108" s="0" t="s">
-        <v>698</v>
+        <v>108</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="0" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
       <c r="B109" s="0" t="b">
         <v>1</v>
@@ -15218,7 +15218,7 @@
     </row>
     <row r="110">
       <c r="A110" s="0" t="s">
-        <v>1155</v>
+        <v>1175</v>
       </c>
       <c r="B110" s="0" t="b">
         <v>1</v>
@@ -15246,7 +15246,7 @@
         <v>1</v>
       </c>
       <c r="C112" s="0" t="s">
-        <v>37</v>
+        <v>698</v>
       </c>
     </row>
     <row r="113">
@@ -15257,7 +15257,7 @@
         <v>1</v>
       </c>
       <c r="C113" s="0" t="s">
-        <v>457</v>
+        <v>698</v>
       </c>
     </row>
     <row r="114">
@@ -15268,7 +15268,7 @@
         <v>1</v>
       </c>
       <c r="C114" s="0" t="s">
-        <v>346</v>
+        <v>698</v>
       </c>
     </row>
     <row r="115">
@@ -15279,7 +15279,7 @@
         <v>1</v>
       </c>
       <c r="C115" s="0" t="s">
-        <v>698</v>
+        <v>29</v>
       </c>
     </row>
     <row r="116">
@@ -15301,7 +15301,7 @@
         <v>1</v>
       </c>
       <c r="C117" s="0" t="s">
-        <v>526</v>
+        <v>698</v>
       </c>
     </row>
     <row r="118">
@@ -15309,7 +15309,7 @@
         <v>1183</v>
       </c>
       <c r="B118" s="0" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C118" s="0" t="s">
         <v>698</v>
@@ -15320,7 +15320,7 @@
         <v>1184</v>
       </c>
       <c r="B119" s="0" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C119" s="0" t="s">
         <v>698</v>
@@ -15331,7 +15331,7 @@
         <v>1185</v>
       </c>
       <c r="B120" s="0" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C120" s="0" t="s">
         <v>698</v>
@@ -15356,7 +15356,7 @@
         <v>1</v>
       </c>
       <c r="C122" s="0" t="s">
-        <v>698</v>
+        <v>564</v>
       </c>
     </row>
     <row r="123">
@@ -15433,7 +15433,7 @@
         <v>1</v>
       </c>
       <c r="C129" s="0" t="s">
-        <v>108</v>
+        <v>698</v>
       </c>
     </row>
     <row r="130">
@@ -15510,7 +15510,7 @@
         <v>1</v>
       </c>
       <c r="C136" s="0" t="s">
-        <v>29</v>
+        <v>698</v>
       </c>
     </row>
     <row r="137">
@@ -15587,7 +15587,7 @@
         <v>1</v>
       </c>
       <c r="C143" s="0" t="s">
-        <v>564</v>
+        <v>698</v>
       </c>
     </row>
     <row r="144">
@@ -15598,7 +15598,7 @@
         <v>1</v>
       </c>
       <c r="C144" s="0" t="s">
-        <v>698</v>
+        <v>238</v>
       </c>
     </row>
     <row r="145">
@@ -15796,7 +15796,7 @@
         <v>1</v>
       </c>
       <c r="C162" s="0" t="s">
-        <v>698</v>
+        <v>462</v>
       </c>
     </row>
     <row r="163">
@@ -15829,7 +15829,7 @@
         <v>1</v>
       </c>
       <c r="C165" s="0" t="s">
-        <v>238</v>
+        <v>698</v>
       </c>
     </row>
     <row r="166">
@@ -15840,7 +15840,7 @@
         <v>1</v>
       </c>
       <c r="C166" s="0" t="s">
-        <v>698</v>
+        <v>284</v>
       </c>
     </row>
     <row r="167">
@@ -15928,7 +15928,7 @@
         <v>1</v>
       </c>
       <c r="C174" s="0" t="s">
-        <v>698</v>
+        <v>188</v>
       </c>
     </row>
     <row r="175">
@@ -16016,7 +16016,7 @@
         <v>1</v>
       </c>
       <c r="C182" s="0" t="s">
-        <v>698</v>
+        <v>4</v>
       </c>
     </row>
     <row r="183">
@@ -16027,7 +16027,7 @@
         <v>1</v>
       </c>
       <c r="C183" s="0" t="s">
-        <v>462</v>
+        <v>698</v>
       </c>
     </row>
     <row r="184">
@@ -16071,7 +16071,7 @@
         <v>1</v>
       </c>
       <c r="C187" s="0" t="s">
-        <v>135</v>
+        <v>698</v>
       </c>
     </row>
     <row r="188">
@@ -16082,7 +16082,7 @@
         <v>1</v>
       </c>
       <c r="C188" s="0" t="s">
-        <v>284</v>
+        <v>698</v>
       </c>
     </row>
     <row r="189">
@@ -16159,7 +16159,7 @@
         <v>1</v>
       </c>
       <c r="C195" s="0" t="s">
-        <v>188</v>
+        <v>698</v>
       </c>
     </row>
     <row r="196">
@@ -16247,7 +16247,7 @@
         <v>1</v>
       </c>
       <c r="C203" s="0" t="s">
-        <v>4</v>
+        <v>698</v>
       </c>
     </row>
     <row r="204">
@@ -16423,7 +16423,7 @@
         <v>1</v>
       </c>
       <c r="C219" s="0" t="s">
-        <v>698</v>
+        <v>52</v>
       </c>
     </row>
     <row r="220">
@@ -16434,7 +16434,7 @@
         <v>1</v>
       </c>
       <c r="C220" s="0" t="s">
-        <v>698</v>
+        <v>52</v>
       </c>
     </row>
     <row r="221">
@@ -16467,7 +16467,7 @@
         <v>1</v>
       </c>
       <c r="C223" s="0" t="s">
-        <v>698</v>
+        <v>372</v>
       </c>
     </row>
     <row r="224">
@@ -16500,7 +16500,7 @@
         <v>1</v>
       </c>
       <c r="C226" s="0" t="s">
-        <v>698</v>
+        <v>218</v>
       </c>
     </row>
     <row r="227">
@@ -16533,7 +16533,7 @@
         <v>1</v>
       </c>
       <c r="C229" s="0" t="s">
-        <v>698</v>
+        <v>135</v>
       </c>
     </row>
     <row r="230">
@@ -16621,7 +16621,7 @@
         <v>1</v>
       </c>
       <c r="C237" s="0" t="s">
-        <v>698</v>
+        <v>218</v>
       </c>
     </row>
     <row r="238">
@@ -16676,7 +16676,7 @@
         <v>1</v>
       </c>
       <c r="C242" s="0" t="s">
-        <v>372</v>
+        <v>540</v>
       </c>
     </row>
     <row r="243">
@@ -16709,7 +16709,7 @@
         <v>1</v>
       </c>
       <c r="C245" s="0" t="s">
-        <v>218</v>
+        <v>698</v>
       </c>
     </row>
     <row r="246">
@@ -16731,7 +16731,7 @@
         <v>1</v>
       </c>
       <c r="C247" s="0" t="s">
-        <v>698</v>
+        <v>149</v>
       </c>
     </row>
     <row r="248">
@@ -16742,7 +16742,7 @@
         <v>1</v>
       </c>
       <c r="C248" s="0" t="s">
-        <v>135</v>
+        <v>698</v>
       </c>
     </row>
     <row r="249">
@@ -16764,7 +16764,7 @@
         <v>1</v>
       </c>
       <c r="C250" s="0" t="s">
-        <v>698</v>
+        <v>4</v>
       </c>
     </row>
     <row r="251">
@@ -16830,7 +16830,7 @@
         <v>1</v>
       </c>
       <c r="C256" s="0" t="s">
-        <v>218</v>
+        <v>698</v>
       </c>
     </row>
     <row r="257">
@@ -16885,7 +16885,7 @@
         <v>1</v>
       </c>
       <c r="C261" s="0" t="s">
-        <v>540</v>
+        <v>698</v>
       </c>
     </row>
     <row r="262">
@@ -16940,7 +16940,7 @@
         <v>1</v>
       </c>
       <c r="C266" s="0" t="s">
-        <v>149</v>
+        <v>698</v>
       </c>
     </row>
     <row r="267">
@@ -16973,7 +16973,7 @@
         <v>1</v>
       </c>
       <c r="C269" s="0" t="s">
-        <v>4</v>
+        <v>141</v>
       </c>
     </row>
     <row r="270">
@@ -17025,7 +17025,7 @@
         <v>1339</v>
       </c>
       <c r="B274" s="0" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C274" s="0" t="s">
         <v>698</v>
@@ -17039,7 +17039,7 @@
         <v>1</v>
       </c>
       <c r="C275" s="0" t="s">
-        <v>698</v>
+        <v>153</v>
       </c>
     </row>
     <row r="276">
@@ -17058,7 +17058,7 @@
         <v>1342</v>
       </c>
       <c r="B277" s="0" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C277" s="0" t="s">
         <v>698</v>
@@ -17069,7 +17069,7 @@
         <v>1343</v>
       </c>
       <c r="B278" s="0" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C278" s="0" t="s">
         <v>698</v>
@@ -17149,7 +17149,7 @@
         <v>1</v>
       </c>
       <c r="C285" s="0" t="s">
-        <v>698</v>
+        <v>147</v>
       </c>
     </row>
     <row r="286">
@@ -17182,7 +17182,7 @@
         <v>1</v>
       </c>
       <c r="C288" s="0" t="s">
-        <v>141</v>
+        <v>698</v>
       </c>
     </row>
     <row r="289">
@@ -17215,7 +17215,7 @@
         <v>1</v>
       </c>
       <c r="C291" s="0" t="s">
-        <v>698</v>
+        <v>346</v>
       </c>
     </row>
     <row r="292">
@@ -17226,7 +17226,7 @@
         <v>1</v>
       </c>
       <c r="C292" s="0" t="s">
-        <v>698</v>
+        <v>164</v>
       </c>
     </row>
     <row r="293">
@@ -17234,7 +17234,7 @@
         <v>1358</v>
       </c>
       <c r="B293" s="0" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C293" s="0" t="s">
         <v>698</v>
@@ -17245,7 +17245,7 @@
         <v>1359</v>
       </c>
       <c r="B294" s="0" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C294" s="0" t="s">
         <v>698</v>
@@ -17300,7 +17300,7 @@
         <v>1364</v>
       </c>
       <c r="B299" s="0" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C299" s="0" t="s">
         <v>698</v>
@@ -17311,7 +17311,7 @@
         <v>1365</v>
       </c>
       <c r="B300" s="0" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C300" s="0" t="s">
         <v>698</v>
@@ -17325,7 +17325,7 @@
         <v>1</v>
       </c>
       <c r="C301" s="0" t="s">
-        <v>147</v>
+        <v>698</v>
       </c>
     </row>
     <row r="302">
@@ -17333,7 +17333,7 @@
         <v>1367</v>
       </c>
       <c r="B302" s="0" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C302" s="0" t="s">
         <v>698</v>
@@ -17344,7 +17344,7 @@
         <v>1368</v>
       </c>
       <c r="B303" s="0" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C303" s="0" t="s">
         <v>698</v>
@@ -17358,7 +17358,7 @@
         <v>1</v>
       </c>
       <c r="C304" s="0" t="s">
-        <v>698</v>
+        <v>288</v>
       </c>
     </row>
     <row r="305">
@@ -17369,7 +17369,7 @@
         <v>1</v>
       </c>
       <c r="C305" s="0" t="s">
-        <v>698</v>
+        <v>37</v>
       </c>
     </row>
     <row r="306">
@@ -17380,7 +17380,7 @@
         <v>1</v>
       </c>
       <c r="C306" s="0" t="s">
-        <v>698</v>
+        <v>677</v>
       </c>
     </row>
     <row r="307">
@@ -17391,7 +17391,7 @@
         <v>1</v>
       </c>
       <c r="C307" s="0" t="s">
-        <v>346</v>
+        <v>698</v>
       </c>
     </row>
     <row r="308">
@@ -17402,7 +17402,7 @@
         <v>1</v>
       </c>
       <c r="C308" s="0" t="s">
-        <v>164</v>
+        <v>698</v>
       </c>
     </row>
     <row r="309">
@@ -17421,7 +17421,7 @@
         <v>1375</v>
       </c>
       <c r="B310" s="0" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C310" s="0" t="s">
         <v>698</v>
@@ -17446,7 +17446,7 @@
         <v>1</v>
       </c>
       <c r="C312" s="0" t="s">
-        <v>698</v>
+        <v>141</v>
       </c>
     </row>
     <row r="313">
@@ -17454,7 +17454,7 @@
         <v>1378</v>
       </c>
       <c r="B313" s="0" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C313" s="0" t="s">
         <v>698</v>
@@ -17479,7 +17479,7 @@
         <v>1</v>
       </c>
       <c r="C315" s="0" t="s">
-        <v>677</v>
+        <v>698</v>
       </c>
     </row>
     <row r="316">
@@ -17509,7 +17509,7 @@
         <v>1383</v>
       </c>
       <c r="B318" s="0" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C318" s="0" t="s">
         <v>698</v>
@@ -17520,7 +17520,7 @@
         <v>1384</v>
       </c>
       <c r="B319" s="0" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C319" s="0" t="s">
         <v>698</v>
@@ -17542,10 +17542,10 @@
         <v>1386</v>
       </c>
       <c r="B321" s="0" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C321" s="0" t="s">
-        <v>141</v>
+        <v>698</v>
       </c>
     </row>
     <row r="322">
@@ -17553,7 +17553,7 @@
         <v>1387</v>
       </c>
       <c r="B322" s="0" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C322" s="0" t="s">
         <v>698</v>
@@ -17567,7 +17567,7 @@
         <v>1</v>
       </c>
       <c r="C323" s="0" t="s">
-        <v>698</v>
+        <v>443</v>
       </c>
     </row>
     <row r="324">
@@ -17600,7 +17600,7 @@
         <v>1</v>
       </c>
       <c r="C326" s="0" t="s">
-        <v>698</v>
+        <v>58</v>
       </c>
     </row>
     <row r="327">
@@ -17655,7 +17655,7 @@
         <v>1</v>
       </c>
       <c r="C331" s="0" t="s">
-        <v>698</v>
+        <v>121</v>
       </c>
     </row>
     <row r="332">
@@ -17666,7 +17666,7 @@
         <v>1</v>
       </c>
       <c r="C332" s="0" t="s">
-        <v>443</v>
+        <v>292</v>
       </c>
     </row>
     <row r="333">
@@ -17699,7 +17699,7 @@
         <v>1</v>
       </c>
       <c r="C335" s="0" t="s">
-        <v>58</v>
+        <v>698</v>
       </c>
     </row>
     <row r="336">
@@ -17721,7 +17721,7 @@
         <v>1</v>
       </c>
       <c r="C337" s="0" t="s">
-        <v>698</v>
+        <v>288</v>
       </c>
     </row>
     <row r="338">
@@ -17754,7 +17754,7 @@
         <v>1</v>
       </c>
       <c r="C340" s="0" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="341">
@@ -17765,7 +17765,7 @@
         <v>1</v>
       </c>
       <c r="C341" s="0" t="s">
-        <v>292</v>
+        <v>159</v>
       </c>
     </row>
     <row r="342">
@@ -17776,7 +17776,7 @@
         <v>1</v>
       </c>
       <c r="C342" s="0" t="s">
-        <v>698</v>
+        <v>169</v>
       </c>
     </row>
     <row r="343">
@@ -17806,7 +17806,7 @@
         <v>1410</v>
       </c>
       <c r="B345" s="0" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C345" s="0" t="s">
         <v>698</v>
@@ -17820,7 +17820,7 @@
         <v>1</v>
       </c>
       <c r="C346" s="0" t="s">
-        <v>288</v>
+        <v>698</v>
       </c>
     </row>
     <row r="347">
@@ -17839,7 +17839,7 @@
         <v>1413</v>
       </c>
       <c r="B348" s="0" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C348" s="0" t="s">
         <v>698</v>
@@ -17853,7 +17853,7 @@
         <v>1</v>
       </c>
       <c r="C349" s="0" t="s">
-        <v>119</v>
+        <v>698</v>
       </c>
     </row>
     <row r="350">
@@ -17864,7 +17864,7 @@
         <v>1</v>
       </c>
       <c r="C350" s="0" t="s">
-        <v>159</v>
+        <v>698</v>
       </c>
     </row>
     <row r="351">
@@ -17875,7 +17875,7 @@
         <v>1</v>
       </c>
       <c r="C351" s="0" t="s">
-        <v>169</v>
+        <v>698</v>
       </c>
     </row>
     <row r="352">
@@ -18007,7 +18007,7 @@
         <v>1</v>
       </c>
       <c r="C363" s="0" t="s">
-        <v>698</v>
+        <v>296</v>
       </c>
     </row>
     <row r="364">
@@ -18062,7 +18062,7 @@
         <v>1</v>
       </c>
       <c r="C368" s="0" t="s">
-        <v>698</v>
+        <v>119</v>
       </c>
     </row>
     <row r="369">
@@ -18106,7 +18106,7 @@
         <v>1</v>
       </c>
       <c r="C372" s="0" t="s">
-        <v>296</v>
+        <v>698</v>
       </c>
     </row>
     <row r="373">
@@ -18128,7 +18128,7 @@
         <v>1</v>
       </c>
       <c r="C374" s="0" t="s">
-        <v>698</v>
+        <v>590</v>
       </c>
     </row>
     <row r="375">
@@ -18136,7 +18136,7 @@
         <v>1440</v>
       </c>
       <c r="B375" s="0" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C375" s="0" t="s">
         <v>698</v>
@@ -18147,7 +18147,7 @@
         <v>1441</v>
       </c>
       <c r="B376" s="0" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C376" s="0" t="s">
         <v>698</v>
@@ -18158,10 +18158,10 @@
         <v>1442</v>
       </c>
       <c r="B377" s="0" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C377" s="0" t="s">
-        <v>119</v>
+        <v>698</v>
       </c>
     </row>
     <row r="378">
@@ -18194,7 +18194,7 @@
         <v>1</v>
       </c>
       <c r="C380" s="0" t="s">
-        <v>698</v>
+        <v>470</v>
       </c>
     </row>
     <row r="381">
@@ -18216,7 +18216,7 @@
         <v>1</v>
       </c>
       <c r="C382" s="0" t="s">
-        <v>698</v>
+        <v>135</v>
       </c>
     </row>
     <row r="383">
@@ -18224,10 +18224,10 @@
         <v>1448</v>
       </c>
       <c r="B383" s="0" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C383" s="0" t="s">
-        <v>590</v>
+        <v>698</v>
       </c>
     </row>
     <row r="384">

</xml_diff>